<commit_message>
English exercises flow change
</commit_message>
<xml_diff>
--- a/docs/StatusTracker.xlsx
+++ b/docs/StatusTracker.xlsx
@@ -1,113 +1,97 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryamirani/Desktop/iiit/sem4/dass/project/project-monorepo-team-20/docs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC16F634-1C50-F840-9C71-6D0C87C4E73B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="620" windowWidth="24740" windowHeight="16100" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
-    <sheet name="Status" sheetId="2" r:id="rId2"/>
+    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Status" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="94">
-  <si>
-    <t>Using the Status tracker</t>
-  </si>
-  <si>
-    <t>At the end of each week, update the status of all activities completed during the week</t>
-  </si>
-  <si>
-    <t>The status tracker shown in this worksheet is an example tracker (values filled are during the middle of the week)</t>
-  </si>
-  <si>
-    <t>Fill in hours spent on each activity during the current week</t>
-  </si>
-  <si>
-    <t>If 5 team members each spent an hour, that counts as 5 hours</t>
-  </si>
-  <si>
-    <t>Fill in time for activities not fully completed ("ongoing") as well, then update these values during following weeks</t>
-  </si>
-  <si>
-    <t>During the planning phases, identify the activities to be done during each week</t>
-  </si>
-  <si>
-    <t>If you spend time on an activity not listed in the tracker, add the activity and list actual hours (need not fill in estimated hours if you didn't estimate it up front)</t>
-  </si>
-  <si>
-    <t>For new activities, identify the type of activity - documentation, coordination, estimation etc.</t>
-  </si>
-  <si>
-    <t>At the end of each week, plan ahead for the following week</t>
-  </si>
-  <si>
-    <t>Identify people responsible for each activity</t>
-  </si>
-  <si>
-    <t>Estimate the hours needed for the activity</t>
-  </si>
-  <si>
-    <t>PROJECT NUMBER</t>
-  </si>
-  <si>
-    <t>PROJECT NAME</t>
-  </si>
-  <si>
-    <t>Slearn</t>
-  </si>
-  <si>
-    <t>PROJECT MENTOR (sponsor)</t>
-  </si>
-  <si>
-    <t>shankar foundation</t>
-  </si>
-  <si>
-    <t>TEAM MEMBERS</t>
-  </si>
-  <si>
-    <t>arya mirani</t>
-  </si>
-  <si>
-    <t>vaishnavi k</t>
-  </si>
-  <si>
-    <t>dev patel</t>
-  </si>
-  <si>
-    <t>manan trivedi</t>
-  </si>
-  <si>
-    <t>vruddhi shah</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+  <si>
+    <t xml:space="preserve">Using the Status tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the end of each week, update the status of all activities completed during the week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The status tracker shown in this worksheet is an example tracker (values filled are during the middle of the week)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill in hours spent on each activity during the current week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If 5 team members each spent an hour, that counts as 5 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill in time for activities not fully completed ("ongoing") as well, then update these values during following weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During the planning phases, identify the activities to be done during each week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you spend time on an activity not listed in the tracker, add the activity and list actual hours (need not fill in estimated hours if you didn't estimate it up front)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For new activities, identify the type of activity - documentation, coordination, estimation etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the end of each week, plan ahead for the following week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify people responsible for each activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimate the hours needed for the activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROJECT NUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROJECT NAME</t>
+  </si>
+  <si>
+    <t>S-Learn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROJECT MENTOR (sponsor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shankar Foundation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM MEMBERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arya Mirani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaishnavi K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev Patel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manan Trivedi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vruddhi Shah</t>
   </si>
   <si>
     <t>Santhosh</t>
   </si>
   <si>
-    <t>Activity Name</t>
+    <t xml:space="preserve">Activity Name</t>
   </si>
   <si>
     <t>Type</t>
@@ -116,10 +100,10 @@
     <t>Responsible</t>
   </si>
   <si>
-    <t>Estimated Team Hours</t>
-  </si>
-  <si>
-    <t>Actual Hours</t>
+    <t xml:space="preserve">Estimated Team Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Hours</t>
   </si>
   <si>
     <t>Status</t>
@@ -128,19 +112,19 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Estimation error</t>
-  </si>
-  <si>
-    <t>Estimation error %</t>
+    <t xml:space="preserve">Estimation error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimation error %</t>
   </si>
   <si>
     <t xml:space="preserve">    See Instructions sheet for usage</t>
   </si>
   <si>
-    <t>Week 1 (January 16-  January 17)</t>
-  </si>
-  <si>
-    <t>[Jan 16] Set a meeting with the client</t>
+    <t xml:space="preserve">Week 1 (January 16-  January 17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Jan 16] Set a meeting with the client</t>
   </si>
   <si>
     <t>Coordination</t>
@@ -152,10 +136,10 @@
     <t>Done</t>
   </si>
   <si>
-    <t>onboarding of the team with the client and knowing the process</t>
-  </si>
-  <si>
-    <t>[Jan 16] Updated design requirements after client meeting</t>
+    <t xml:space="preserve">onboarding of the team with the client and knowing the process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Jan 16] Updated design requirements after client meeting</t>
   </si>
   <si>
     <t>Documentation</t>
@@ -164,25 +148,28 @@
     <t>vaishnavi</t>
   </si>
   <si>
-    <t>update the design requirements according to client feedback, and divide work among team members</t>
-  </si>
-  <si>
-    <t>Week 2 (January 18 - January  24)</t>
-  </si>
-  <si>
-    <t>[jan 18] restructure repository</t>
-  </si>
-  <si>
-    <t>setup branches and connect to vercel</t>
-  </si>
-  <si>
-    <t>[jan 18] changes requested by client in meeting</t>
-  </si>
-  <si>
-    <t>UI changes</t>
-  </si>
-  <si>
-    <t>[jan 19] changes requested by client in meeting</t>
+    <t xml:space="preserve">update the design requirements according to client feedback, and divide work among team members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 2 (January 18 - January  24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[jan 18] restructure repository</t>
+  </si>
+  <si>
+    <t>Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">setup branches and connect to vercel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[jan 18] changes requested by client in meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[jan 19] changes requested by client in meeting</t>
   </si>
   <si>
     <t>manan</t>
@@ -194,193 +181,182 @@
     <t>vruddhi</t>
   </si>
   <si>
-    <t>[jan 21] restructer the sidebar, other ui improvements</t>
+    <t xml:space="preserve">[jan 21] restructer the sidebar, other ui improvements</t>
   </si>
   <si>
     <t>dev</t>
   </si>
   <si>
-    <t>[Jan 22] client requested changes – color changes, navigation changes between vocabulary exercises</t>
-  </si>
-  <si>
-    <t>[jan 23] Pushed the code to vercel for sending to clients, made website responsive for phone and tablet</t>
-  </si>
-  <si>
-    <t>Meeting 2 with client [Jan 23]</t>
+    <t xml:space="preserve">[Jan 22] client requested changes – color changes, navigation changes between vocabulary exercises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[jan 23] Pushed the code to vercel for sending to clients, made website responsive for phone and tablet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting 2 with client [Jan 23]</t>
   </si>
   <si>
     <t>all</t>
   </si>
   <si>
-    <t>updated client on changes made; documented feedback to further changes</t>
-  </si>
-  <si>
-    <t>Week 3 (January 25 – January 31)</t>
-  </si>
-  <si>
-    <t>allocated work in implementing further modules</t>
-  </si>
-  <si>
-    <t>dev, vruddhi ,manan, vaishnavi</t>
-  </si>
-  <si>
-    <t>project synopsis</t>
-  </si>
-  <si>
-    <t>Week 4(Feb 1 - Feb 7)</t>
-  </si>
-  <si>
-    <t>[Feb 1]  make backend database using supabase</t>
+    <t xml:space="preserve">updated client on changes made; documented feedback to further changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 3 (January 25 – January 31)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allocated work in implementing further modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dev, vruddhi ,manan, vaishnavi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project synopsis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 4(Feb 1 - Feb 7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Feb 1]  make backend database using supabase</t>
   </si>
   <si>
     <t>Ongoing</t>
   </si>
   <si>
-    <t>[Feb 1] created new modules – evs</t>
-  </si>
-  <si>
-    <t>[feb 2] created new modules – english</t>
-  </si>
-  <si>
-    <t>add new modules in English</t>
-  </si>
-  <si>
-    <t>[feb 2-3] created new modules (math word problems, english read words), added exercises to evs module</t>
-  </si>
-  <si>
-    <t>[feb 3] Team Internal meeting</t>
-  </si>
-  <si>
-    <t>Discussed navigation issues and variations in module implementation; resplit tasks to ensure uniformity among modules</t>
+    <t xml:space="preserve">[Feb 1] created new modules – evs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 2] created new modules – english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add new modules in English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 2-3] created new modules (math word problems, english read words), added exercises to evs module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 3] Team Internal meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussed navigation issues and variations in module implementation; resplit tasks to ensure uniformity among modules</t>
   </si>
   <si>
     <t xml:space="preserve">[feb 3] created new modules - english </t>
   </si>
   <si>
-    <t>[feb 3] refactored and organized codebase for vercel and grade-wise navigation</t>
-  </si>
-  <si>
-    <t>navigation changes – dashboard</t>
-  </si>
-  <si>
-    <t>Go to Shankar Foundation School [Feb 4]</t>
+    <t xml:space="preserve">[feb 3] refactored and organized codebase for vercel and grade-wise navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigation changes – dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to Shankar Foundation School [Feb 4]</t>
   </si>
   <si>
     <t>All</t>
   </si>
   <si>
-    <t>visited the school and saw the process of teaching</t>
-  </si>
-  <si>
-    <t>[feb 5] main page dropdown menus, navigation between modules</t>
-  </si>
-  <si>
-    <t>added dropdown menu  for the grades on the main page  which further nevigates to the menu of specific subject of that grade and which will nevigate to exersices of that subject .</t>
-  </si>
-  <si>
-    <t>Further exercise changes in modules – english</t>
-  </si>
-  <si>
-    <t>exercise changes in modules – math</t>
-  </si>
-  <si>
-    <t>[feb 7] resizing and rearranging evs</t>
-  </si>
-  <si>
-    <t>Week 5 (Feb 8 – Feb 14)</t>
-  </si>
-  <si>
-    <t>Updating project plan, updating status tracker since first meet</t>
-  </si>
-  <si>
-    <t>[Feb 11] Computer module fixes requested by client</t>
-  </si>
-  <si>
-    <t>Development</t>
+    <t xml:space="preserve">visited the school and saw the process of teaching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 5] main page dropdown menus, navigation between modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added dropdown menu  for the grades on the main page  which further nevigates to the menu of specific subject of that grade and which will nevigate to exersices of that subject .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further exercise changes in modules – english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exercise changes in modules – math</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 7] resizing and rearranging evs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 5 (Feb 8 – Feb 14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating project plan, updating status tracker since first meet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Feb 11] Computer module fixes requested by client</t>
   </si>
   <si>
     <t>Dev</t>
   </si>
   <si>
-    <t>Week 6 (Feb 15 – Feb 21)</t>
-  </si>
-  <si>
-    <t>check the backend and frontend connection</t>
+    <t xml:space="preserve">[feb 10] meeting with sachin sir </t>
+  </si>
+  <si>
+    <t xml:space="preserve">add pages for login, singup, teachers, parents, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check the backend and frontend connection</t>
   </si>
   <si>
     <t>Testing</t>
   </si>
   <si>
-    <t xml:space="preserve">[feb 10] meeting with sachin sir </t>
-  </si>
-  <si>
-    <t>add pages for login, singup, teachers, parents, etc.</t>
+    <t xml:space="preserve">Week 6 (Feb 15 – Feb 21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI Improvements for home pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed flow of English exercise</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9">
     <font>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <u/>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <color rgb="FF0000D4"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="14.000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="14.000000"/>
       <color indexed="4"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="14.000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="12.000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
       <b/>
       <u/>
-      <sz val="12"/>
+      <sz val="12.000000"/>
       <color rgb="FF0000D4"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color theme="1"/>
+      <sz val="10.000000"/>
       <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -417,92 +393,95 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+  <cellXfs count="31">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="2" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="6" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="7" fillId="4" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="6" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="7" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="6" fillId="4" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -510,41 +489,7 @@
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCF305"/>
-          <bgColor rgb="FFFCF305"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF006411"/>
-          <bgColor rgb="FF006411"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDD0806"/>
-          <bgColor rgb="FFDD0806"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -557,8 +502,291 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -610,7 +838,7 @@
         <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -724,90 +952,88 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0">
-      <selection activeCell="A30" sqref="A30"/>
+    <sheetView topLeftCell="A15" zoomScale="110" workbookViewId="0">
+      <selection activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="50.33203125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="88.33203125"/>
+    <col customWidth="1" min="2" max="2" width="50.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" ht="18">
       <c r="A1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" ht="18">
       <c r="A2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15">
       <c r="B15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" ht="30.75" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -815,7 +1041,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" ht="25.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -823,7 +1049,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" ht="25.5" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -831,7 +1057,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" ht="37.5" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -839,83 +1065,84 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" ht="18">
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" ht="18">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" ht="18">
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" ht="18">
       <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" ht="18">
       <c r="B27" s="3"/>
     </row>
   </sheetData>
+  <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51181102362204689" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I240"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="110" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView zoomScale="110" workbookViewId="0">
+      <selection activeCell="C52" activeCellId="0" sqref="C52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="42" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="3" max="3" width="13.33203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="48.33203125" customWidth="1"/>
-    <col min="8" max="9" width="11.33203125" style="5" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="42"/>
+    <col customWidth="1" min="2" max="2" width="47.6640625"/>
+    <col customWidth="1" min="3" max="3" style="1" width="13.33203125"/>
+    <col customWidth="1" min="4" max="4" style="1" width="11"/>
+    <col customWidth="1" min="5" max="5" style="1" width="11.33203125"/>
+    <col customWidth="1" min="6" max="6" style="4" width="12.33203125"/>
+    <col customWidth="1" min="7" max="7" width="48.33203125"/>
+    <col customWidth="1" min="8" max="9" style="5" width="11.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="24.75" customHeight="1">
       <c r="A1" s="2" t="str">
         <f>(Instructions!A19)</f>
-        <v>PROJECT NUMBER</v>
+        <v xml:space="preserve">PROJECT NUMBER</v>
       </c>
       <c r="B1" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" ht="25.5" customHeight="1">
       <c r="A2" s="2" t="str">
         <f>(Instructions!A20)</f>
-        <v>PROJECT NAME</v>
+        <v xml:space="preserve">PROJECT NAME</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="30.75" customHeight="1">
       <c r="A3" s="2" t="str">
         <f>(Instructions!A21)</f>
-        <v>PROJECT MENTOR (sponsor)</v>
+        <v xml:space="preserve">PROJECT MENTOR (sponsor)</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="7" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" s="7" customFormat="1" ht="38.25">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -944,7 +1171,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="6" s="13" customFormat="1" ht="30.75" customHeight="1" outlineLevel="2">
       <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
@@ -955,7 +1182,7 @@
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="7" outlineLevel="2">
       <c r="A7" s="17" t="s">
         <v>34</v>
       </c>
@@ -974,7 +1201,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="8" outlineLevel="2">
       <c r="A8" s="23" t="s">
         <v>35</v>
       </c>
@@ -1005,7 +1232,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="9" outlineLevel="2">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1029,27 +1256,27 @@
       </c>
       <c r="H9" s="22">
         <f t="shared" si="0"/>
-        <v>-5.0000000000000044E-2</v>
+        <v>-0.050000000000000044</v>
       </c>
       <c r="I9" s="22">
         <f t="shared" si="1"/>
         <v>4.7619047619047654</v>
       </c>
     </row>
-    <row r="10" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="10" outlineLevel="2">
       <c r="A10" s="25"/>
       <c r="B10" s="1"/>
       <c r="C10" s="24"/>
       <c r="H10" s="22" t="str">
-        <f t="shared" ref="H10:H75" si="2">IF(OR(D10="",E10=""),"",D10-E10)</f>
+        <f t="shared" ref="H10:H73" si="2">IF(OR(D10="",E10=""),"",D10-E10)</f>
         <v/>
       </c>
       <c r="I10" s="22" t="str">
-        <f t="shared" ref="I10:I75" si="3">IF(OR(H10="",E10=0),"",ABS(H10)/E10*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="18" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
+        <f t="shared" ref="I10:I73" si="3">IF(OR(H10="",E10=0),"",ABS(H10)/E10*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" s="18" customFormat="1" outlineLevel="2">
       <c r="A11" s="17" t="s">
         <v>44</v>
       </c>
@@ -1066,12 +1293,12 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="12" ht="14" outlineLevel="2">
       <c r="A12" s="25" t="s">
         <v>45</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C12" s="24" t="s">
         <v>37</v>
@@ -1086,23 +1313,23 @@
         <v>38</v>
       </c>
       <c r="G12" t="s">
+        <v>47</v>
+      </c>
+      <c r="H12" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I12" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" s="18" customFormat="1" ht="14" outlineLevel="2">
+      <c r="A13" s="25" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="H12" s="22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I12" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="18" customFormat="1" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
-      <c r="A13" s="25" t="s">
-        <v>47</v>
-      </c>
-      <c r="B13" s="28" t="s">
-        <v>87</v>
       </c>
       <c r="C13" s="24" t="s">
         <v>37</v>
@@ -1117,7 +1344,7 @@
         <v>38</v>
       </c>
       <c r="G13" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H13" s="22">
         <f t="shared" si="2"/>
@@ -1128,15 +1355,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="18" customFormat="1" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="14" s="18" customFormat="1" ht="14" outlineLevel="2">
       <c r="A14" s="25" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="28" t="s">
-        <v>87</v>
+        <v>50</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C14" s="24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
@@ -1144,7 +1371,7 @@
         <v>38</v>
       </c>
       <c r="G14" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H14" s="22" t="str">
         <f t="shared" si="2"/>
@@ -1155,15 +1382,15 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:9" s="18" customFormat="1" ht="42" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="15" s="18" customFormat="1" ht="38.25" outlineLevel="2">
       <c r="A15" s="25" t="s">
-        <v>51</v>
-      </c>
-      <c r="B15" s="28" t="s">
-        <v>87</v>
+        <v>52</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C15" s="24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D15" s="1">
         <v>1</v>
@@ -1175,7 +1402,7 @@
         <v>38</v>
       </c>
       <c r="G15" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H15" s="22">
         <f t="shared" si="2"/>
@@ -1186,15 +1413,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="18" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="16" s="18" customFormat="1" ht="25.5" outlineLevel="2">
       <c r="A16" s="25" t="s">
-        <v>53</v>
-      </c>
-      <c r="B16" s="28" t="s">
-        <v>87</v>
+        <v>54</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C16" s="24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
@@ -1202,7 +1429,7 @@
         <v>38</v>
       </c>
       <c r="G16" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H16" s="22" t="str">
         <f t="shared" si="2"/>
@@ -1213,12 +1440,12 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="17" s="18" customFormat="1" ht="38.25" outlineLevel="2">
       <c r="A17" s="25" t="s">
-        <v>55</v>
-      </c>
-      <c r="B17" s="28" t="s">
-        <v>87</v>
+        <v>56</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>46</v>
       </c>
       <c r="C17" s="24" t="s">
         <v>42</v>
@@ -1233,7 +1460,7 @@
         <v>38</v>
       </c>
       <c r="G17" s="18" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H17" s="22">
         <f t="shared" si="2"/>
@@ -1244,12 +1471,12 @@
         <v>63.636363636363633</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="42" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="18" ht="38.25" outlineLevel="2">
       <c r="A18" s="25" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="B18" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>37</v>
@@ -1272,15 +1499,15 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="19" ht="14" outlineLevel="2">
       <c r="A19" s="25" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D19" s="1">
         <v>1</v>
@@ -1292,7 +1519,7 @@
         <v>38</v>
       </c>
       <c r="G19" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H19" s="22">
         <f t="shared" si="2"/>
@@ -1303,7 +1530,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="20" outlineLevel="2">
       <c r="A20" s="25"/>
       <c r="B20" s="1"/>
       <c r="H20" s="22" t="str">
@@ -1315,9 +1542,9 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" s="18" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="21" s="18" customFormat="1" outlineLevel="2">
       <c r="A21" s="17" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C21" s="19"/>
       <c r="D21" s="19"/>
@@ -1332,15 +1559,15 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22">
       <c r="A22" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D22" s="1">
         <v>1</v>
@@ -1360,15 +1587,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23">
       <c r="A23" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>41</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F23" s="4" t="s">
         <v>38</v>
@@ -1382,7 +1609,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24">
       <c r="H24" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1392,9 +1619,9 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25">
       <c r="A25" s="17" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="B25" s="18"/>
       <c r="C25" s="19"/>
@@ -1411,12 +1638,12 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26">
       <c r="A26" s="23" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B26" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C26" s="1" t="s">
         <v>37</v>
@@ -1425,7 +1652,7 @@
         <v>10</v>
       </c>
       <c r="F26" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H26" s="22" t="str">
         <f t="shared" si="2"/>
@@ -1436,15 +1663,15 @@
         <v/>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27">
       <c r="A27" s="23" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C27" s="24" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F27" s="26" t="s">
         <v>38</v>
@@ -1459,15 +1686,15 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28">
       <c r="A28" s="23" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C28" s="24" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D28" s="1">
         <v>2</v>
@@ -1479,7 +1706,7 @@
         <v>38</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H28" s="22">
         <f t="shared" si="2"/>
@@ -1490,12 +1717,12 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="29">
       <c r="A29" s="23" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="B29" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C29" s="24" t="s">
         <v>42</v>
@@ -1519,15 +1746,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30">
       <c r="A30" s="23" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C30" s="24" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="D30" s="1">
         <v>2</v>
@@ -1539,7 +1766,7 @@
         <v>38</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H30" s="22">
         <f t="shared" si="2"/>
@@ -1550,15 +1777,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="31">
       <c r="A31" s="23" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B31" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C31" s="24" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F31" s="4" t="s">
         <v>38</v>
@@ -1573,15 +1800,15 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32">
       <c r="A32" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F32" s="4" t="s">
         <v>38</v>
@@ -1595,15 +1822,15 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33">
       <c r="A33" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C33" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F33" s="4" t="s">
         <v>38</v>
@@ -1617,15 +1844,15 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34">
       <c r="A34" s="23" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="D34" s="1">
         <v>2</v>
@@ -1637,7 +1864,7 @@
         <v>38</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="H34" s="22">
         <f t="shared" si="2"/>
@@ -1648,15 +1875,15 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="35">
       <c r="A35" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C35" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="D35" s="1">
         <v>1</v>
@@ -1668,7 +1895,7 @@
         <v>38</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="H35" s="22">
         <f t="shared" si="2"/>
@@ -1679,15 +1906,15 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="36">
       <c r="A36" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="B36" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C36" s="1" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="F36" s="4" t="s">
         <v>38</v>
@@ -1701,12 +1928,12 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37">
       <c r="A37" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B37" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C37" s="1" t="s">
         <v>37</v>
@@ -1729,15 +1956,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="38">
       <c r="A38" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C38" s="1" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="F38" s="4" t="s">
         <v>38</v>
@@ -1751,7 +1978,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39">
       <c r="B39" s="1"/>
       <c r="H39" s="22" t="str">
         <f t="shared" si="2"/>
@@ -1762,9 +1989,9 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="40">
       <c r="A40" s="17" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="19"/>
@@ -1781,9 +2008,9 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41">
       <c r="A41" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>41</v>
@@ -1794,8 +2021,8 @@
       <c r="D41" s="1">
         <v>3</v>
       </c>
-      <c r="F41" s="29" t="s">
-        <v>66</v>
+      <c r="F41" s="27" t="s">
+        <v>67</v>
       </c>
       <c r="H41" s="22" t="str">
         <f t="shared" si="2"/>
@@ -1806,12 +2033,12 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42">
       <c r="A42" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B42" s="1" t="s">
-        <v>87</v>
+        <v>46</v>
       </c>
       <c r="C42" s="1" t="s">
         <v>88</v>
@@ -1820,29 +2047,29 @@
         <v>0.5</v>
       </c>
       <c r="E42" s="1">
-        <v>0.2</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H42" s="22">
         <f t="shared" si="2"/>
-        <v>0.3</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="I42" s="22">
         <f t="shared" si="3"/>
         <v>149.99999999999997</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A43" s="27" t="s">
-        <v>92</v>
+    <row r="43">
+      <c r="A43" s="28" t="s">
+        <v>89</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C43" s="28" t="s">
-        <v>58</v>
+      <c r="C43" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D43" s="1">
         <v>1.5</v>
@@ -1856,14 +2083,14 @@
       <c r="H43" s="22"/>
       <c r="I43" s="22"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A44" s="27" t="s">
-        <v>93</v>
+    <row r="44">
+      <c r="A44" s="28" t="s">
+        <v>90</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C44" s="28" t="s">
+        <v>46</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D44" s="1">
@@ -1878,15 +2105,15 @@
       <c r="H44" s="22"/>
       <c r="I44" s="22"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A45" s="27" t="s">
-        <v>90</v>
+    <row r="45">
+      <c r="A45" s="28" t="s">
+        <v>91</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="C45" s="28" t="s">
-        <v>58</v>
+        <v>92</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>59</v>
       </c>
       <c r="D45" s="1">
         <v>3</v>
@@ -1895,7 +2122,7 @@
         <v>3</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="H45" s="22">
         <f t="shared" si="2"/>
@@ -1906,9 +2133,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46">
       <c r="A46" s="17" t="s">
-        <v>89</v>
+        <v>93</v>
       </c>
       <c r="B46" s="18"/>
       <c r="C46" s="19"/>
@@ -1925,27 +2152,63 @@
         <v/>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H47" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I47" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H48" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I48" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="49" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="47">
+      <c r="A47" t="s">
+        <v>94</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+      <c r="C47" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D47" s="1">
+        <v>4</v>
+      </c>
+      <c r="E47" s="1">
+        <v>6</v>
+      </c>
+      <c r="F47" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="H47" s="22">
+        <f t="shared" si="2"/>
+        <v>-2</v>
+      </c>
+      <c r="I47" s="22">
+        <f t="shared" si="3"/>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="s">
+        <v>95</v>
+      </c>
+      <c r="B48" t="s">
+        <v>46</v>
+      </c>
+      <c r="C48" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D48" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="E48" s="1">
+        <v>1</v>
+      </c>
+      <c r="F48" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H48" s="22">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="I48" s="22">
+        <f t="shared" si="3"/>
+        <v>50</v>
+      </c>
+    </row>
+    <row r="49">
       <c r="H49" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1955,7 +2218,7 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="50">
       <c r="H50" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1965,7 +2228,7 @@
         <v/>
       </c>
     </row>
-    <row r="51" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="51">
       <c r="H51" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1975,7 +2238,7 @@
         <v/>
       </c>
     </row>
-    <row r="52" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="52">
       <c r="H52" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1985,7 +2248,7 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="53">
       <c r="H53" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1995,7 +2258,7 @@
         <v/>
       </c>
     </row>
-    <row r="54" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="54">
       <c r="H54" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2005,7 +2268,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="55">
       <c r="H55" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2015,7 +2278,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="56">
       <c r="H56" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2025,7 +2288,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="57">
       <c r="H57" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2035,7 +2298,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="58">
       <c r="H58" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2045,7 +2308,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="59">
       <c r="H59" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2055,7 +2318,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="60">
       <c r="H60" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2065,7 +2328,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="61">
       <c r="H61" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2075,7 +2338,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="62">
       <c r="H62" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2085,7 +2348,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="63">
       <c r="H63" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2095,7 +2358,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="64">
       <c r="H64" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2105,7 +2368,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="65">
       <c r="H65" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2115,7 +2378,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="66">
       <c r="H66" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2125,7 +2388,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="67">
       <c r="H67" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2135,7 +2398,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="68">
       <c r="H68" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2145,7 +2408,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="69">
       <c r="H69" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2155,7 +2418,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="70">
       <c r="H70" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2165,7 +2428,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="71">
       <c r="H71" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2175,7 +2438,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="72">
       <c r="H72" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2185,7 +2448,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="73">
       <c r="H73" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2195,37 +2458,37 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="74">
       <c r="H74" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H74:H101" si="4">IF(OR(D74="",E74=""),"",D74-E74)</f>
         <v/>
       </c>
       <c r="I74" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" ref="I74:I101" si="5">IF(OR(H74="",E74=0),"",ABS(H74)/E74*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75">
       <c r="H75" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I75" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76">
       <c r="H76" s="22" t="str">
-        <f t="shared" ref="H76:H101" si="4">IF(OR(D76="",E76=""),"",D76-E76)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I76" s="22" t="str">
-        <f t="shared" ref="I76:I101" si="5">IF(OR(H76="",E76=0),"",ABS(H76)/E76*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="77">
       <c r="H77" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2235,7 +2498,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="78">
       <c r="H78" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2245,7 +2508,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="79">
       <c r="H79" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2255,7 +2518,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="80">
       <c r="H80" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2265,7 +2528,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="81">
       <c r="H81" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2275,7 +2538,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="82">
       <c r="H82" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2285,7 +2548,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="83">
       <c r="H83" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2295,7 +2558,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="84">
       <c r="H84" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2305,7 +2568,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="85">
       <c r="H85" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2315,7 +2578,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="86">
       <c r="H86" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2325,7 +2588,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="87">
       <c r="H87" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2335,7 +2598,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="88">
       <c r="H88" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2345,7 +2608,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="89">
       <c r="H89" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2355,7 +2618,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="90">
       <c r="H90" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2365,7 +2628,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="91">
       <c r="H91" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2375,7 +2638,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="92">
       <c r="H92" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2385,7 +2648,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="93">
       <c r="H93" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2395,7 +2658,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="94">
       <c r="H94" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2405,7 +2668,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="95">
       <c r="H95" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2415,7 +2678,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="96">
       <c r="H96" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2425,7 +2688,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="97">
       <c r="H97" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2435,7 +2698,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="98">
       <c r="H98" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2445,7 +2708,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="99">
       <c r="H99" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2455,7 +2718,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="100">
       <c r="H100" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2465,7 +2728,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="101">
       <c r="H101" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2475,7 +2738,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="102">
       <c r="H102" s="22" t="str">
         <f t="shared" ref="H102:H165" si="6">IF(OR(D102="",E102=""),"",D102-E102)</f>
         <v/>
@@ -2485,7 +2748,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="103">
       <c r="H103" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2495,7 +2758,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="104">
       <c r="H104" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2505,7 +2768,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="105">
       <c r="H105" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2515,7 +2778,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="106">
       <c r="H106" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2525,7 +2788,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="107">
       <c r="H107" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2535,7 +2798,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="108">
       <c r="H108" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2545,7 +2808,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="109">
       <c r="H109" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2555,7 +2818,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="110">
       <c r="H110" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2565,7 +2828,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="111">
       <c r="H111" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2575,7 +2838,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="112">
       <c r="H112" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2585,7 +2848,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="113">
       <c r="H113" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2595,7 +2858,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="114">
       <c r="H114" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2605,7 +2868,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="115">
       <c r="H115" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2615,7 +2878,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="116">
       <c r="H116" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2625,7 +2888,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="117">
       <c r="H117" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2635,7 +2898,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="118">
       <c r="H118" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2645,7 +2908,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="119">
       <c r="H119" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2655,7 +2918,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="120">
       <c r="H120" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2665,7 +2928,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="121">
       <c r="H121" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2675,7 +2938,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="122">
       <c r="H122" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2685,7 +2948,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="123">
       <c r="H123" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2695,7 +2958,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="124">
       <c r="H124" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2705,7 +2968,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="125">
       <c r="H125" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2715,7 +2978,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="126">
       <c r="H126" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2725,7 +2988,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="127">
       <c r="H127" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2735,7 +2998,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="128">
       <c r="H128" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2745,7 +3008,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="129">
       <c r="H129" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2755,7 +3018,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="130">
       <c r="H130" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2765,7 +3028,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="131">
       <c r="H131" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2775,7 +3038,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="132">
       <c r="H132" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2785,7 +3048,7 @@
         <v/>
       </c>
     </row>
-    <row r="133" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="133">
       <c r="H133" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2795,7 +3058,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="134">
       <c r="H134" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2805,7 +3068,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="135">
       <c r="H135" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2815,7 +3078,7 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="136">
       <c r="H136" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2825,7 +3088,7 @@
         <v/>
       </c>
     </row>
-    <row r="137" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="137">
       <c r="H137" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2835,7 +3098,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="138">
       <c r="H138" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2845,7 +3108,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="139">
       <c r="H139" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2855,7 +3118,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="140">
       <c r="H140" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2865,7 +3128,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="141">
       <c r="H141" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2875,7 +3138,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="142">
       <c r="H142" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2885,7 +3148,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="143">
       <c r="H143" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2895,7 +3158,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="144">
       <c r="H144" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2905,7 +3168,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="145">
       <c r="H145" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2915,7 +3178,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="146">
       <c r="H146" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2925,7 +3188,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="147">
       <c r="H147" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2935,7 +3198,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="148">
       <c r="H148" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2945,7 +3208,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="149">
       <c r="H149" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2955,7 +3218,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="150">
       <c r="H150" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2965,7 +3228,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="151">
       <c r="H151" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2975,7 +3238,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="152">
       <c r="H152" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2985,7 +3248,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="153">
       <c r="H153" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2995,7 +3258,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="154">
       <c r="H154" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3005,7 +3268,7 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="155">
       <c r="H155" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3015,7 +3278,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="156">
       <c r="H156" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3025,7 +3288,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="157">
       <c r="H157" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3035,7 +3298,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="158">
       <c r="H158" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3045,7 +3308,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="159">
       <c r="H159" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3055,7 +3318,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="160">
       <c r="H160" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3065,7 +3328,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="161">
       <c r="H161" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3075,7 +3338,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="162">
       <c r="H162" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3085,7 +3348,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="163">
       <c r="H163" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3095,7 +3358,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="164">
       <c r="H164" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3105,7 +3368,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="165">
       <c r="H165" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3115,7 +3378,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="166">
       <c r="H166" s="22" t="str">
         <f t="shared" ref="H166:H229" si="8">IF(OR(D166="",E166=""),"",D166-E166)</f>
         <v/>
@@ -3125,7 +3388,7 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="167">
       <c r="H167" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3135,7 +3398,7 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="168">
       <c r="H168" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3145,7 +3408,7 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="169">
       <c r="H169" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3155,7 +3418,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="170">
       <c r="H170" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3165,7 +3428,7 @@
         <v/>
       </c>
     </row>
-    <row r="171" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="171">
       <c r="H171" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3175,7 +3438,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="172">
       <c r="H172" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3185,7 +3448,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="173">
       <c r="H173" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3195,7 +3458,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="174">
       <c r="H174" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3205,7 +3468,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="175">
       <c r="H175" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3215,7 +3478,7 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="176">
       <c r="H176" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3225,7 +3488,7 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="177">
       <c r="H177" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3235,7 +3498,7 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="178">
       <c r="H178" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3245,7 +3508,7 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="179">
       <c r="H179" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3255,7 +3518,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="180">
       <c r="H180" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3265,7 +3528,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="181">
       <c r="H181" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3275,7 +3538,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="182">
       <c r="H182" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3285,7 +3548,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="183">
       <c r="H183" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3295,7 +3558,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="184">
       <c r="H184" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3305,7 +3568,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="185">
       <c r="H185" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3315,7 +3578,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="186">
       <c r="H186" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3325,7 +3588,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="187">
       <c r="H187" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3335,7 +3598,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="188">
       <c r="H188" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3345,7 +3608,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="189">
       <c r="H189" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3355,7 +3618,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="190">
       <c r="H190" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3365,7 +3628,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="191">
       <c r="H191" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3375,7 +3638,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="192">
       <c r="H192" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3385,7 +3648,7 @@
         <v/>
       </c>
     </row>
-    <row r="193" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="193">
       <c r="H193" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3395,7 +3658,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="194">
       <c r="H194" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3405,7 +3668,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="195">
       <c r="H195" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3415,7 +3678,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="196">
       <c r="H196" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3425,7 +3688,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="197">
       <c r="H197" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3435,7 +3698,7 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="198">
       <c r="H198" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3445,7 +3708,7 @@
         <v/>
       </c>
     </row>
-    <row r="199" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="199">
       <c r="H199" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3455,7 +3718,7 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="200">
       <c r="H200" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3465,7 +3728,7 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="201">
       <c r="H201" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3475,7 +3738,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="202">
       <c r="H202" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3485,7 +3748,7 @@
         <v/>
       </c>
     </row>
-    <row r="203" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="203">
       <c r="H203" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3495,7 +3758,7 @@
         <v/>
       </c>
     </row>
-    <row r="204" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="204">
       <c r="H204" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3505,7 +3768,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="205">
       <c r="H205" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3515,7 +3778,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="206">
       <c r="H206" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3525,7 +3788,7 @@
         <v/>
       </c>
     </row>
-    <row r="207" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="207">
       <c r="H207" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3535,7 +3798,7 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="208">
       <c r="H208" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3545,7 +3808,7 @@
         <v/>
       </c>
     </row>
-    <row r="209" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="209">
       <c r="H209" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3555,7 +3818,7 @@
         <v/>
       </c>
     </row>
-    <row r="210" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="210">
       <c r="H210" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3565,7 +3828,7 @@
         <v/>
       </c>
     </row>
-    <row r="211" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="211">
       <c r="H211" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3575,7 +3838,7 @@
         <v/>
       </c>
     </row>
-    <row r="212" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="212">
       <c r="H212" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3585,7 +3848,7 @@
         <v/>
       </c>
     </row>
-    <row r="213" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="213">
       <c r="H213" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3595,7 +3858,7 @@
         <v/>
       </c>
     </row>
-    <row r="214" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="214">
       <c r="H214" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3605,7 +3868,7 @@
         <v/>
       </c>
     </row>
-    <row r="215" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="215">
       <c r="H215" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3615,7 +3878,7 @@
         <v/>
       </c>
     </row>
-    <row r="216" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="216">
       <c r="H216" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3625,7 +3888,7 @@
         <v/>
       </c>
     </row>
-    <row r="217" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="217">
       <c r="H217" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3635,7 +3898,7 @@
         <v/>
       </c>
     </row>
-    <row r="218" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="218">
       <c r="H218" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3645,7 +3908,7 @@
         <v/>
       </c>
     </row>
-    <row r="219" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="219">
       <c r="H219" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3655,7 +3918,7 @@
         <v/>
       </c>
     </row>
-    <row r="220" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="220">
       <c r="H220" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3665,7 +3928,7 @@
         <v/>
       </c>
     </row>
-    <row r="221" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="221">
       <c r="H221" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3675,7 +3938,7 @@
         <v/>
       </c>
     </row>
-    <row r="222" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="222">
       <c r="H222" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3685,7 +3948,7 @@
         <v/>
       </c>
     </row>
-    <row r="223" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="223">
       <c r="H223" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3695,7 +3958,7 @@
         <v/>
       </c>
     </row>
-    <row r="224" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="224">
       <c r="H224" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3705,7 +3968,7 @@
         <v/>
       </c>
     </row>
-    <row r="225" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="225">
       <c r="H225" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3715,7 +3978,7 @@
         <v/>
       </c>
     </row>
-    <row r="226" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="226">
       <c r="H226" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3725,7 +3988,7 @@
         <v/>
       </c>
     </row>
-    <row r="227" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="227">
       <c r="H227" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3735,7 +3998,7 @@
         <v/>
       </c>
     </row>
-    <row r="228" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="228">
       <c r="H228" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3745,7 +4008,7 @@
         <v/>
       </c>
     </row>
-    <row r="229" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="229">
       <c r="H229" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3755,7 +4018,7 @@
         <v/>
       </c>
     </row>
-    <row r="230" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="230">
       <c r="H230" s="22" t="str">
         <f t="shared" ref="H230:H233" si="10">IF(OR(D230="",E230=""),"",D230-E230)</f>
         <v/>
@@ -3765,7 +4028,7 @@
         <v/>
       </c>
     </row>
-    <row r="231" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="231">
       <c r="H231" s="22" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -3775,7 +4038,7 @@
         <v/>
       </c>
     </row>
-    <row r="232" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="232">
       <c r="H232" s="22" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -3785,7 +4048,7 @@
         <v/>
       </c>
     </row>
-    <row r="233" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="233">
       <c r="H233" s="22" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -3795,78 +4058,136 @@
         <v/>
       </c>
     </row>
-    <row r="234" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="234">
       <c r="I234" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="235" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="235">
       <c r="I235" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="236" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="236">
       <c r="I236" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="237" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="237">
       <c r="I237" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="238" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="238">
       <c r="I238" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="239" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="239">
       <c r="I239" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="240" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="240">
       <c r="I240" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F5:F40 F42:F65520">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Delayed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"Ongoing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F5:F40 F42:F1240" xr:uid="{00B900BB-004E-41B4-824E-003A00B000A4}">
-      <formula1>"Planned,Ongoing,Delayed,Done"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B5:B9 B11:B12 B18:B25 B34 B40:B1240" xr:uid="{00380039-0026-4098-937B-00A4004C0095}">
-      <formula1>"Requirements,Design,Development,Testing,Preparation,Coordination,Documentation,Interfaces,Delivery"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" location="Instructions!A1" display="    See Instructions sheet for usage" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink location="Instructions!A1" ref="A6"/>
   </hyperlinks>
-  <printOptions gridLines="1"/>
+  <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.51181102362204689"/>
-  <pageSetup scale="70" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="70" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter>
     <oddHeader>&amp;LEdit the Header with Your Team ID&amp;C&amp;F&amp;R&amp;D</oddHeader>
   </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{0044009A-00A6-4771-B86B-002300A000A7}">
+            <xm:f>"Delayed"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFDD0806"/>
+                  <bgColor rgb="FFDD0806"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F5:F40 F42:F65520</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00360045-0078-4754-851B-009D0068008E}">
+            <xm:f>"Done"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF006411"/>
+                  <bgColor rgb="FF006411"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F5:F40 F42:F65520</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00A3005F-00C0-49F8-AA0B-0063007E00F9}">
+            <xm:f>"Ongoing"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFCF305"/>
+                  <bgColor rgb="FFFCF305"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F5:F40 F42:F65520</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
+        <x14:dataValidation xr:uid="{00900005-00E8-4DE8-8D5F-001D0094004C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+          <x14:formula1>
+            <xm:f>"Planned,Ongoing,Delayed,Done"</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>F5:F40 F42:F1240</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{005C003E-008F-4DCE-A606-00F500280088}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+          <x14:formula1>
+            <xm:f>"Requirements,Design,Development,Testing,Preparation,Coordination,Documentation,Interfaces,Delivery"</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>B5:B9 B11:B12 B18:B25 B34 B40:B1240</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fixed audio for English exercies
</commit_message>
<xml_diff>
--- a/docs/StatusTracker.xlsx
+++ b/docs/StatusTracker.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="0"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
   <si>
     <t xml:space="preserve">Using the Status tracker</t>
   </si>
@@ -305,6 +305,9 @@
   </si>
   <si>
     <t xml:space="preserve">Changed flow of English exercise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audio clips for English words</t>
   </si>
 </sst>
 </file>
@@ -962,19 +965,19 @@
       <selection activeCell="A30" activeCellId="0" sqref="A30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
   <cols>
     <col customWidth="1" min="1" max="1" width="88.33203125"/>
     <col customWidth="1" min="2" max="2" width="50.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" ht="18">
+    <row r="1" ht="16.5">
       <c r="A1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="18">
+    <row r="2" ht="16.5">
       <c r="A2" s="1"/>
       <c r="C2" s="2"/>
     </row>
@@ -1065,27 +1068,27 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" ht="18">
+    <row r="23" ht="16.5">
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" ht="18">
+    <row r="24" ht="16.5">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" ht="18">
+    <row r="25" ht="16.5">
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" ht="18">
+    <row r="26" ht="16.5">
       <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" ht="18">
+    <row r="27" ht="16.5">
       <c r="B27" s="3"/>
     </row>
   </sheetData>
@@ -1099,7 +1102,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView zoomScale="110" workbookViewId="0">
+    <sheetView topLeftCell="A33" zoomScale="110" workbookViewId="0">
       <selection activeCell="C52" activeCellId="0" sqref="C52"/>
     </sheetView>
   </sheetViews>
@@ -2159,7 +2162,7 @@
       <c r="B47" t="s">
         <v>46</v>
       </c>
-      <c r="C47" s="29" t="s">
+      <c r="C47" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D47" s="1">
@@ -2187,35 +2190,53 @@
       <c r="B48" t="s">
         <v>46</v>
       </c>
-      <c r="C48" s="29" t="s">
+      <c r="C48" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D48" s="1">
+        <v>1</v>
+      </c>
+      <c r="E48" s="1">
         <v>0.5</v>
       </c>
-      <c r="E48" s="1">
+      <c r="F48" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H48" s="22">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="I48" s="22">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="s">
+        <v>96</v>
+      </c>
+      <c r="B49" t="s">
+        <v>46</v>
+      </c>
+      <c r="C49" s="29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D49" s="1">
         <v>1</v>
       </c>
-      <c r="F48" s="30" t="s">
+      <c r="E49" s="1">
+        <v>0.75</v>
+      </c>
+      <c r="F49" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="H48" s="22">
-        <f t="shared" si="2"/>
-        <v>-0.5</v>
-      </c>
-      <c r="I48" s="22">
-        <f t="shared" si="3"/>
-        <v>50</v>
-      </c>
-    </row>
-    <row r="49">
-      <c r="H49" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I49" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
+      <c r="H49" s="22">
+        <f t="shared" si="2"/>
+        <v>0.25</v>
+      </c>
+      <c r="I49" s="22">
+        <f t="shared" si="3"/>
+        <v>33.333333333333329</v>
       </c>
     </row>
     <row r="50">
@@ -4114,7 +4135,7 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
       <x14:conditionalFormattings>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{0044009A-00A6-4771-B86B-002300A000A7}">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{003200B5-006B-481F-BD7A-007000D500DA}">
             <xm:f>"Delayed"</xm:f>
             <x14:dxf>
               <font>
@@ -4131,7 +4152,7 @@
           <xm:sqref>F5:F40 F42:F65520</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00360045-0078-4754-851B-009D0068008E}">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00F00075-000D-42E6-B430-00F7007200B3}">
             <xm:f>"Done"</xm:f>
             <x14:dxf>
               <font>
@@ -4148,7 +4169,7 @@
           <xm:sqref>F5:F40 F42:F65520</xm:sqref>
         </x14:conditionalFormatting>
         <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{00A3005F-00C0-49F8-AA0B-0063007E00F9}">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{009000C3-0040-47E9-B89A-00B2002E0052}">
             <xm:f>"Ongoing"</xm:f>
             <x14:dxf>
               <font>
@@ -4168,7 +4189,7 @@
     </ext>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{00900005-00E8-4DE8-8D5F-001D0094004C}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{004C0068-0053-4772-9BC1-008500B300EB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Planned,Ongoing,Delayed,Done"</xm:f>
           </x14:formula1>
@@ -4177,7 +4198,7 @@
           </x14:formula2>
           <xm:sqref>F5:F40 F42:F1240</xm:sqref>
         </x14:dataValidation>
-        <x14:dataValidation xr:uid="{005C003E-008F-4DCE-A606-00F500280088}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+        <x14:dataValidation xr:uid="{00F60079-004C-4143-A0AF-009700D80028}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
           <x14:formula1>
             <xm:f>"Requirements,Design,Development,Testing,Preparation,Coordination,Documentation,Interfaces,Delivery"</xm:f>
           </x14:formula1>

</xml_diff>

<commit_message>
workflow changes, comp. module changes, status tracker also updated
</commit_message>
<xml_diff>
--- a/docs/StatusTracker.xlsx
+++ b/docs/StatusTracker.xlsx
@@ -1,97 +1,113 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryamirani/Desktop/iiit/sem4/dass/project/project-monorepo-team-20/docs/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A8F3AE-1AFF-544A-A4FC-A850E505325C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="620" windowWidth="38780" windowHeight="23580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Status" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
+    <sheet name="Status" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr iterateDelta="0.0001"/>
+  <calcPr calcId="191029" iterateDelta="1E-4"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="97">
-  <si>
-    <t xml:space="preserve">Using the Status tracker</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At the end of each week, update the status of all activities completed during the week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">The status tracker shown in this worksheet is an example tracker (values filled are during the middle of the week)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fill in hours spent on each activity during the current week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If 5 team members each spent an hour, that counts as 5 hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Fill in time for activities not fully completed ("ongoing") as well, then update these values during following weeks</t>
-  </si>
-  <si>
-    <t xml:space="preserve">During the planning phases, identify the activities to be done during each week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">If you spend time on an activity not listed in the tracker, add the activity and list actual hours (need not fill in estimated hours if you didn't estimate it up front)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">For new activities, identify the type of activity - documentation, coordination, estimation etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">At the end of each week, plan ahead for the following week</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Identify people responsible for each activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimate the hours needed for the activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROJECT NUMBER</t>
-  </si>
-  <si>
-    <t xml:space="preserve">PROJECT NAME</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="100">
+  <si>
+    <t>Using the Status tracker</t>
+  </si>
+  <si>
+    <t>At the end of each week, update the status of all activities completed during the week</t>
+  </si>
+  <si>
+    <t>The status tracker shown in this worksheet is an example tracker (values filled are during the middle of the week)</t>
+  </si>
+  <si>
+    <t>Fill in hours spent on each activity during the current week</t>
+  </si>
+  <si>
+    <t>If 5 team members each spent an hour, that counts as 5 hours</t>
+  </si>
+  <si>
+    <t>Fill in time for activities not fully completed ("ongoing") as well, then update these values during following weeks</t>
+  </si>
+  <si>
+    <t>During the planning phases, identify the activities to be done during each week</t>
+  </si>
+  <si>
+    <t>If you spend time on an activity not listed in the tracker, add the activity and list actual hours (need not fill in estimated hours if you didn't estimate it up front)</t>
+  </si>
+  <si>
+    <t>For new activities, identify the type of activity - documentation, coordination, estimation etc.</t>
+  </si>
+  <si>
+    <t>At the end of each week, plan ahead for the following week</t>
+  </si>
+  <si>
+    <t>Identify people responsible for each activity</t>
+  </si>
+  <si>
+    <t>Estimate the hours needed for the activity</t>
+  </si>
+  <si>
+    <t>PROJECT NUMBER</t>
+  </si>
+  <si>
+    <t>PROJECT NAME</t>
   </si>
   <si>
     <t>S-Learn</t>
   </si>
   <si>
-    <t xml:space="preserve">PROJECT MENTOR (sponsor)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Shankar Foundation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEAM MEMBERS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Arya Mirani</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vaishnavi K</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dev Patel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Manan Trivedi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Vruddhi Shah</t>
+    <t>PROJECT MENTOR (sponsor)</t>
+  </si>
+  <si>
+    <t>Shankar Foundation</t>
+  </si>
+  <si>
+    <t>TEAM MEMBERS</t>
+  </si>
+  <si>
+    <t>Arya Mirani</t>
+  </si>
+  <si>
+    <t>Vaishnavi K</t>
+  </si>
+  <si>
+    <t>Dev Patel</t>
+  </si>
+  <si>
+    <t>Manan Trivedi</t>
+  </si>
+  <si>
+    <t>Vruddhi Shah</t>
   </si>
   <si>
     <t>Santhosh</t>
   </si>
   <si>
-    <t xml:space="preserve">Activity Name</t>
+    <t>Activity Name</t>
   </si>
   <si>
     <t>Type</t>
@@ -100,10 +116,10 @@
     <t>Responsible</t>
   </si>
   <si>
-    <t xml:space="preserve">Estimated Team Hours</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Actual Hours</t>
+    <t>Estimated Team Hours</t>
+  </si>
+  <si>
+    <t>Actual Hours</t>
   </si>
   <si>
     <t>Status</t>
@@ -112,19 +128,19 @@
     <t>Comments</t>
   </si>
   <si>
-    <t xml:space="preserve">Estimation error</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Estimation error %</t>
+    <t>Estimation error</t>
+  </si>
+  <si>
+    <t>Estimation error %</t>
   </si>
   <si>
     <t xml:space="preserve">    See Instructions sheet for usage</t>
   </si>
   <si>
-    <t xml:space="preserve">Week 1 (January 16-  January 17)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Jan 16] Set a meeting with the client</t>
+    <t>Week 1 (January 16-  January 17)</t>
+  </si>
+  <si>
+    <t>[Jan 16] Set a meeting with the client</t>
   </si>
   <si>
     <t>Coordination</t>
@@ -136,10 +152,10 @@
     <t>Done</t>
   </si>
   <si>
-    <t xml:space="preserve">onboarding of the team with the client and knowing the process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Jan 16] Updated design requirements after client meeting</t>
+    <t>onboarding of the team with the client and knowing the process</t>
+  </si>
+  <si>
+    <t>[Jan 16] Updated design requirements after client meeting</t>
   </si>
   <si>
     <t>Documentation</t>
@@ -148,28 +164,28 @@
     <t>vaishnavi</t>
   </si>
   <si>
-    <t xml:space="preserve">update the design requirements according to client feedback, and divide work among team members</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 2 (January 18 - January  24)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[jan 18] restructure repository</t>
+    <t>update the design requirements according to client feedback, and divide work among team members</t>
+  </si>
+  <si>
+    <t>Week 2 (January 18 - January  24)</t>
+  </si>
+  <si>
+    <t>[jan 18] restructure repository</t>
   </si>
   <si>
     <t>Development</t>
   </si>
   <si>
-    <t xml:space="preserve">setup branches and connect to vercel</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[jan 18] changes requested by client in meeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UI changes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[jan 19] changes requested by client in meeting</t>
+    <t>setup branches and connect to vercel</t>
+  </si>
+  <si>
+    <t>[jan 18] changes requested by client in meeting</t>
+  </si>
+  <si>
+    <t>UI changes</t>
+  </si>
+  <si>
+    <t>[jan 19] changes requested by client in meeting</t>
   </si>
   <si>
     <t>manan</t>
@@ -181,106 +197,106 @@
     <t>vruddhi</t>
   </si>
   <si>
-    <t xml:space="preserve">[jan 21] restructer the sidebar, other ui improvements</t>
+    <t>[jan 21] restructer the sidebar, other ui improvements</t>
   </si>
   <si>
     <t>dev</t>
   </si>
   <si>
-    <t xml:space="preserve">[Jan 22] client requested changes – color changes, navigation changes between vocabulary exercises</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[jan 23] Pushed the code to vercel for sending to clients, made website responsive for phone and tablet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Meeting 2 with client [Jan 23]</t>
+    <t>[Jan 22] client requested changes – color changes, navigation changes between vocabulary exercises</t>
+  </si>
+  <si>
+    <t>[jan 23] Pushed the code to vercel for sending to clients, made website responsive for phone and tablet</t>
+  </si>
+  <si>
+    <t>Meeting 2 with client [Jan 23]</t>
   </si>
   <si>
     <t>all</t>
   </si>
   <si>
-    <t xml:space="preserve">updated client on changes made; documented feedback to further changes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 3 (January 25 – January 31)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">allocated work in implementing further modules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">dev, vruddhi ,manan, vaishnavi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">project synopsis</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 4(Feb 1 - Feb 7)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Feb 1]  make backend database using supabase</t>
+    <t>updated client on changes made; documented feedback to further changes</t>
+  </si>
+  <si>
+    <t>Week 3 (January 25 – January 31)</t>
+  </si>
+  <si>
+    <t>allocated work in implementing further modules</t>
+  </si>
+  <si>
+    <t>dev, vruddhi ,manan, vaishnavi</t>
+  </si>
+  <si>
+    <t>project synopsis</t>
+  </si>
+  <si>
+    <t>Week 4(Feb 1 - Feb 7)</t>
+  </si>
+  <si>
+    <t>[Feb 1]  make backend database using supabase</t>
   </si>
   <si>
     <t>Ongoing</t>
   </si>
   <si>
-    <t xml:space="preserve">[Feb 1] created new modules – evs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[feb 2] created new modules – english</t>
-  </si>
-  <si>
-    <t xml:space="preserve">add new modules in English</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[feb 2-3] created new modules (math word problems, english read words), added exercises to evs module</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[feb 3] Team Internal meeting</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Discussed navigation issues and variations in module implementation; resplit tasks to ensure uniformity among modules</t>
+    <t>[Feb 1] created new modules – evs</t>
+  </si>
+  <si>
+    <t>[feb 2] created new modules – english</t>
+  </si>
+  <si>
+    <t>add new modules in English</t>
+  </si>
+  <si>
+    <t>[feb 2-3] created new modules (math word problems, english read words), added exercises to evs module</t>
+  </si>
+  <si>
+    <t>[feb 3] Team Internal meeting</t>
+  </si>
+  <si>
+    <t>Discussed navigation issues and variations in module implementation; resplit tasks to ensure uniformity among modules</t>
   </si>
   <si>
     <t xml:space="preserve">[feb 3] created new modules - english </t>
   </si>
   <si>
-    <t xml:space="preserve">[feb 3] refactored and organized codebase for vercel and grade-wise navigation</t>
-  </si>
-  <si>
-    <t xml:space="preserve">navigation changes – dashboard</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Go to Shankar Foundation School [Feb 4]</t>
+    <t>[feb 3] refactored and organized codebase for vercel and grade-wise navigation</t>
+  </si>
+  <si>
+    <t>navigation changes – dashboard</t>
+  </si>
+  <si>
+    <t>Go to Shankar Foundation School [Feb 4]</t>
   </si>
   <si>
     <t>All</t>
   </si>
   <si>
-    <t xml:space="preserve">visited the school and saw the process of teaching</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[feb 5] main page dropdown menus, navigation between modules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">added dropdown menu  for the grades on the main page  which further nevigates to the menu of specific subject of that grade and which will nevigate to exersices of that subject .</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Further exercise changes in modules – english</t>
-  </si>
-  <si>
-    <t xml:space="preserve">exercise changes in modules – math</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[feb 7] resizing and rearranging evs</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Week 5 (Feb 8 – Feb 14)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Updating project plan, updating status tracker since first meet</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[Feb 11] Computer module fixes requested by client</t>
+    <t>visited the school and saw the process of teaching</t>
+  </si>
+  <si>
+    <t>[feb 5] main page dropdown menus, navigation between modules</t>
+  </si>
+  <si>
+    <t>added dropdown menu  for the grades on the main page  which further nevigates to the menu of specific subject of that grade and which will nevigate to exersices of that subject .</t>
+  </si>
+  <si>
+    <t>Further exercise changes in modules – english</t>
+  </si>
+  <si>
+    <t>exercise changes in modules – math</t>
+  </si>
+  <si>
+    <t>[feb 7] resizing and rearranging evs</t>
+  </si>
+  <si>
+    <t>Week 5 (Feb 8 – Feb 14)</t>
+  </si>
+  <si>
+    <t>Updating project plan, updating status tracker since first meet</t>
+  </si>
+  <si>
+    <t>[Feb 11] Computer module fixes requested by client</t>
   </si>
   <si>
     <t>Dev</t>
@@ -289,77 +305,97 @@
     <t xml:space="preserve">[feb 10] meeting with sachin sir </t>
   </si>
   <si>
-    <t xml:space="preserve">add pages for login, singup, teachers, parents, etc.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">check the backend and frontend connection</t>
+    <t>add pages for login, singup, teachers, parents, etc.</t>
+  </si>
+  <si>
+    <t>check the backend and frontend connection</t>
   </si>
   <si>
     <t>Testing</t>
   </si>
   <si>
-    <t xml:space="preserve">Week 6 (Feb 15 – Feb 21)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">UI Improvements for home pages</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Changed flow of English exercise</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Audio clips for English words</t>
+    <t>Week 6 (Feb 15 – Feb 21)</t>
+  </si>
+  <si>
+    <t>UI Improvements for home pages</t>
+  </si>
+  <si>
+    <t>Changed flow of English exercise</t>
+  </si>
+  <si>
+    <t>Audio clips for English words</t>
+  </si>
+  <si>
+    <t>Fixed the overall flow of the entire modules</t>
+  </si>
+  <si>
+    <t>connect the frontend to the backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">push the new pages (backend + audiio) to vercel, test the workflow </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="9">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
-      <sz val="10.000000"/>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10.000000"/>
+      <sz val="10"/>
       <color rgb="FF0000D4"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="14.000000"/>
+      <sz val="14"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="14.000000"/>
+      <sz val="14"/>
       <color indexed="4"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="14.000000"/>
+      <sz val="14"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10.000000"/>
+      <sz val="10"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12.000000"/>
+      <sz val="12"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <u/>
-      <sz val="12.000000"/>
+      <sz val="12"/>
       <color rgb="FF0000D4"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10.000000"/>
+      <sz val="10"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -396,104 +432,141 @@
   </fills>
   <borders count="1">
     <border>
-      <left style="none"/>
-      <right style="none"/>
-      <top style="none"/>
-      <bottom style="none"/>
-      <diagonal style="none"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf fontId="6" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="7" fillId="4" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf fontId="6" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="6" fillId="4" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="5" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
-    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFCF305"/>
+          <bgColor rgb="FFFCF305"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF006411"/>
+          <bgColor rgb="FF006411"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFDD0806"/>
+          <bgColor rgb="FFDD0806"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FF00FA00"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -505,291 +578,8 @@
 </styleSheet>
 </file>
 
-<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
-  <a:themeElements>
-    <a:clrScheme name="Office">
-      <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
-      </a:dk1>
-      <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
-      </a:lt1>
-      <a:dk2>
-        <a:srgbClr val="1F497D"/>
-      </a:dk2>
-      <a:lt2>
-        <a:srgbClr val="EEECE1"/>
-      </a:lt2>
-      <a:accent1>
-        <a:srgbClr val="4F81BD"/>
-      </a:accent1>
-      <a:accent2>
-        <a:srgbClr val="C0504D"/>
-      </a:accent2>
-      <a:accent3>
-        <a:srgbClr val="9BBB59"/>
-      </a:accent3>
-      <a:accent4>
-        <a:srgbClr val="8064A2"/>
-      </a:accent4>
-      <a:accent5>
-        <a:srgbClr val="4BACC6"/>
-      </a:accent5>
-      <a:accent6>
-        <a:srgbClr val="F79646"/>
-      </a:accent6>
-      <a:hlink>
-        <a:srgbClr val="0000FF"/>
-      </a:hlink>
-      <a:folHlink>
-        <a:srgbClr val="800080"/>
-      </a:folHlink>
-    </a:clrScheme>
-    <a:fontScheme name="Office">
-      <a:majorFont>
-        <a:latin typeface="Cambria"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Angsana New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:majorFont>
-      <a:minorFont>
-        <a:latin typeface="Calibri"/>
-        <a:ea typeface=""/>
-        <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Cordia New"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-      </a:minorFont>
-    </a:fontScheme>
-    <a:fmtScheme name="Office">
-      <a:fillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="50000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="35000">
-              <a:schemeClr val="phClr">
-                <a:tint val="37000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:tint val="15000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:shade val="51000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="80000">
-              <a:schemeClr val="phClr">
-                <a:shade val="93000"/>
-                <a:satMod val="130000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="94000"/>
-                <a:satMod val="135000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:lin ang="16200000" scaled="0"/>
-        </a:gradFill>
-      </a:fillStyleLst>
-      <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr">
-              <a:shade val="95000"/>
-              <a:satMod val="105000"/>
-            </a:schemeClr>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
-          <a:solidFill>
-            <a:schemeClr val="phClr"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-        </a:ln>
-      </a:lnStyleLst>
-      <a:effectStyleLst>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="38000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-        </a:effectStyle>
-        <a:effectStyle>
-          <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
-              <a:srgbClr val="000000">
-                <a:alpha val="35000"/>
-              </a:srgbClr>
-            </a:outerShdw>
-          </a:effectLst>
-          <a:scene3d>
-            <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
-            </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
-            </a:lightRig>
-          </a:scene3d>
-          <a:sp3d>
-            <a:bevelT w="63500" h="25400"/>
-          </a:sp3d>
-        </a:effectStyle>
-      </a:effectStyleLst>
-      <a:bgFillStyleLst>
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="40000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="40000">
-              <a:schemeClr val="phClr">
-                <a:tint val="45000"/>
-                <a:shade val="99000"/>
-                <a:satMod val="350000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="20000"/>
-                <a:satMod val="255000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
-          </a:path>
-        </a:gradFill>
-        <a:gradFill rotWithShape="1">
-          <a:gsLst>
-            <a:gs pos="0">
-              <a:schemeClr val="phClr">
-                <a:tint val="80000"/>
-                <a:satMod val="300000"/>
-              </a:schemeClr>
-            </a:gs>
-            <a:gs pos="100000">
-              <a:schemeClr val="phClr">
-                <a:shade val="30000"/>
-                <a:satMod val="200000"/>
-              </a:schemeClr>
-            </a:gs>
-          </a:gsLst>
-          <a:path path="circle">
-            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
-          </a:path>
-        </a:gradFill>
-      </a:bgFillStyleLst>
-    </a:fmtScheme>
-  </a:themeElements>
-  <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
-</a:theme>
-</file>
-
-<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -841,7 +631,7 @@
         <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="">
+    <a:fmtScheme>
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -955,88 +745,90 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView topLeftCell="A15" zoomScale="110" workbookViewId="0">
-      <selection activeCell="A30" activeCellId="0" sqref="A30"/>
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="88.33203125"/>
-    <col customWidth="1" min="2" max="2" width="50.33203125"/>
+    <col min="1" max="1" width="88.33203125" customWidth="1"/>
+    <col min="2" max="2" width="50.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="16.5">
+    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="16.5">
+    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
       <c r="B15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" ht="30.75" customHeight="1">
+    <row r="19" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -1044,7 +836,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" ht="25.5" customHeight="1">
+    <row r="20" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -1052,7 +844,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" ht="25.5" customHeight="1">
+    <row r="21" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -1060,7 +852,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" ht="37.5" customHeight="1">
+    <row r="22" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -1068,84 +860,83 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" ht="16.5">
+    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" ht="16.5">
+    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" ht="16.5">
+    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" ht="16.5">
+    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" ht="16.5">
+    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
       <c r="B27" s="3"/>
     </row>
   </sheetData>
-  <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51181102362204689" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+  <dimension ref="A1:I241"/>
   <sheetViews>
-    <sheetView topLeftCell="A33" zoomScale="110" workbookViewId="0">
-      <selection activeCell="C52" activeCellId="0" sqref="C52"/>
+    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" outlineLevelRow="2"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
   <cols>
-    <col customWidth="1" min="1" max="1" width="42"/>
-    <col customWidth="1" min="2" max="2" width="47.6640625"/>
-    <col customWidth="1" min="3" max="3" style="1" width="13.33203125"/>
-    <col customWidth="1" min="4" max="4" style="1" width="11"/>
-    <col customWidth="1" min="5" max="5" style="1" width="11.33203125"/>
-    <col customWidth="1" min="6" max="6" style="4" width="12.33203125"/>
-    <col customWidth="1" min="7" max="7" width="48.33203125"/>
-    <col customWidth="1" min="8" max="9" style="5" width="11.33203125"/>
+    <col min="1" max="1" width="50.5" customWidth="1"/>
+    <col min="2" max="2" width="47.6640625" customWidth="1"/>
+    <col min="3" max="3" width="41.83203125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11" style="1" customWidth="1"/>
+    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
+    <col min="6" max="6" width="12.33203125" style="4" customWidth="1"/>
+    <col min="7" max="7" width="48.33203125" customWidth="1"/>
+    <col min="8" max="9" width="11.33203125" style="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="24.75" customHeight="1">
+    <row r="1" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="2" t="str">
         <f>(Instructions!A19)</f>
-        <v xml:space="preserve">PROJECT NUMBER</v>
+        <v>PROJECT NUMBER</v>
       </c>
       <c r="B1" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="2" ht="25.5" customHeight="1">
+    <row r="2" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="str">
         <f>(Instructions!A20)</f>
-        <v xml:space="preserve">PROJECT NAME</v>
+        <v>PROJECT NAME</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" ht="30.75" customHeight="1">
+    <row r="3" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="str">
         <f>(Instructions!A21)</f>
-        <v xml:space="preserve">PROJECT MENTOR (sponsor)</v>
+        <v>PROJECT MENTOR (sponsor)</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" s="7" customFormat="1" ht="38.25">
+    <row r="5" spans="1:9" s="7" customFormat="1" ht="28" x14ac:dyDescent="0.15">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -1174,7 +965,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" s="13" customFormat="1" ht="30.75" customHeight="1" outlineLevel="2">
+    <row r="6" spans="1:9" s="13" customFormat="1" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
@@ -1185,7 +976,7 @@
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" outlineLevel="2">
+    <row r="7" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A7" s="17" t="s">
         <v>34</v>
       </c>
@@ -1204,7 +995,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" outlineLevel="2">
+    <row r="8" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A8" s="23" t="s">
         <v>35</v>
       </c>
@@ -1235,7 +1026,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" outlineLevel="2">
+    <row r="9" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1259,27 +1050,27 @@
       </c>
       <c r="H9" s="22">
         <f t="shared" si="0"/>
-        <v>-0.050000000000000044</v>
+        <v>-5.0000000000000044E-2</v>
       </c>
       <c r="I9" s="22">
         <f t="shared" si="1"/>
         <v>4.7619047619047654</v>
       </c>
     </row>
-    <row r="10" outlineLevel="2">
+    <row r="10" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A10" s="25"/>
       <c r="B10" s="1"/>
       <c r="C10" s="24"/>
       <c r="H10" s="22" t="str">
-        <f t="shared" ref="H10:H73" si="2">IF(OR(D10="",E10=""),"",D10-E10)</f>
+        <f t="shared" ref="H10:H74" si="2">IF(OR(D10="",E10=""),"",D10-E10)</f>
         <v/>
       </c>
       <c r="I10" s="22" t="str">
-        <f t="shared" ref="I10:I73" si="3">IF(OR(H10="",E10=0),"",ABS(H10)/E10*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" s="18" customFormat="1" outlineLevel="2">
+        <f t="shared" ref="I10:I74" si="3">IF(OR(H10="",E10=0),"",ABS(H10)/E10*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" spans="1:9" s="18" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A11" s="17" t="s">
         <v>44</v>
       </c>
@@ -1296,7 +1087,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" ht="14" outlineLevel="2">
+    <row r="12" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A12" s="25" t="s">
         <v>45</v>
       </c>
@@ -1327,7 +1118,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" s="18" customFormat="1" ht="14" outlineLevel="2">
+    <row r="13" spans="1:9" s="18" customFormat="1" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A13" s="25" t="s">
         <v>48</v>
       </c>
@@ -1358,7 +1149,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" s="18" customFormat="1" ht="14" outlineLevel="2">
+    <row r="14" spans="1:9" s="18" customFormat="1" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A14" s="25" t="s">
         <v>50</v>
       </c>
@@ -1385,7 +1176,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" s="18" customFormat="1" ht="38.25" outlineLevel="2">
+    <row r="15" spans="1:9" s="18" customFormat="1" ht="42" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A15" s="25" t="s">
         <v>52</v>
       </c>
@@ -1416,7 +1207,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" s="18" customFormat="1" ht="25.5" outlineLevel="2">
+    <row r="16" spans="1:9" s="18" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A16" s="25" t="s">
         <v>54</v>
       </c>
@@ -1443,7 +1234,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" s="18" customFormat="1" ht="38.25" outlineLevel="2">
+    <row r="17" spans="1:9" s="18" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A17" s="25" t="s">
         <v>56</v>
       </c>
@@ -1474,7 +1265,7 @@
         <v>63.636363636363633</v>
       </c>
     </row>
-    <row r="18" ht="38.25" outlineLevel="2">
+    <row r="18" spans="1:9" ht="42" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A18" s="25" t="s">
         <v>57</v>
       </c>
@@ -1502,7 +1293,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" ht="14" outlineLevel="2">
+    <row r="19" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A19" s="25" t="s">
         <v>58</v>
       </c>
@@ -1533,7 +1324,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" outlineLevel="2">
+    <row r="20" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A20" s="25"/>
       <c r="B20" s="1"/>
       <c r="H20" s="22" t="str">
@@ -1545,7 +1336,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" s="18" customFormat="1" outlineLevel="2">
+    <row r="21" spans="1:9" s="18" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
       <c r="A21" s="17" t="s">
         <v>61</v>
       </c>
@@ -1562,7 +1353,7 @@
         <v/>
       </c>
     </row>
-    <row r="22">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1590,7 +1381,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1612,7 +1403,7 @@
         <v/>
       </c>
     </row>
-    <row r="24">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H24" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1622,7 +1413,7 @@
         <v/>
       </c>
     </row>
-    <row r="25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A25" s="17" t="s">
         <v>65</v>
       </c>
@@ -1641,7 +1432,7 @@
         <v/>
       </c>
     </row>
-    <row r="26">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A26" s="23" t="s">
         <v>66</v>
       </c>
@@ -1654,19 +1445,22 @@
       <c r="D26" s="1">
         <v>10</v>
       </c>
+      <c r="E26" s="1">
+        <v>11</v>
+      </c>
       <c r="F26" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H26" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I26" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="27">
+        <v>38</v>
+      </c>
+      <c r="H26" s="22">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="I26" s="22">
+        <f t="shared" si="3"/>
+        <v>9.0909090909090917</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A27" s="23" t="s">
         <v>68</v>
       </c>
@@ -1689,7 +1483,7 @@
         <v/>
       </c>
     </row>
-    <row r="28">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A28" s="23" t="s">
         <v>69</v>
       </c>
@@ -1720,8 +1514,8 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="29">
-      <c r="A29" s="23" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A29" s="30" t="s">
         <v>71</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -1749,7 +1543,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A30" s="23" t="s">
         <v>72</v>
       </c>
@@ -1780,7 +1574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A31" s="23" t="s">
         <v>74</v>
       </c>
@@ -1803,7 +1597,7 @@
         <v/>
       </c>
     </row>
-    <row r="32">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A32" t="s">
         <v>75</v>
       </c>
@@ -1825,7 +1619,7 @@
         <v/>
       </c>
     </row>
-    <row r="33">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A33" t="s">
         <v>76</v>
       </c>
@@ -1847,7 +1641,7 @@
         <v/>
       </c>
     </row>
-    <row r="34">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A34" s="23" t="s">
         <v>77</v>
       </c>
@@ -1878,7 +1672,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A35" t="s">
         <v>80</v>
       </c>
@@ -1909,7 +1703,7 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="36">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A36" t="s">
         <v>82</v>
       </c>
@@ -1931,7 +1725,7 @@
         <v/>
       </c>
     </row>
-    <row r="37">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A37" t="s">
         <v>83</v>
       </c>
@@ -1959,7 +1753,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A38" t="s">
         <v>84</v>
       </c>
@@ -1981,7 +1775,7 @@
         <v/>
       </c>
     </row>
-    <row r="39">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
       <c r="B39" s="1"/>
       <c r="H39" s="22" t="str">
         <f t="shared" si="2"/>
@@ -1992,7 +1786,7 @@
         <v/>
       </c>
     </row>
-    <row r="40">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A40" s="17" t="s">
         <v>85</v>
       </c>
@@ -2011,7 +1805,7 @@
         <v/>
       </c>
     </row>
-    <row r="41">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A41" t="s">
         <v>86</v>
       </c>
@@ -2036,71 +1830,75 @@
         <v/>
       </c>
     </row>
-    <row r="42">
-      <c r="A42" t="s">
-        <v>87</v>
+    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A42" s="28" t="s">
+        <v>98</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="1" t="s">
-        <v>88</v>
+      <c r="C42" s="29" t="s">
+        <v>37</v>
       </c>
       <c r="D42" s="1">
-        <v>0.5</v>
+        <v>3</v>
       </c>
       <c r="E42" s="1">
-        <v>0.20000000000000001</v>
+        <v>3</v>
       </c>
       <c r="F42" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H42" s="22">
-        <f t="shared" si="2"/>
-        <v>0.29999999999999999</v>
+        <v>0</v>
       </c>
       <c r="I42" s="22">
-        <f t="shared" si="3"/>
-        <v>149.99999999999997</v>
-      </c>
-    </row>
-    <row r="43">
-      <c r="A43" s="28" t="s">
-        <v>89</v>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A43" t="s">
+        <v>87</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>59</v>
+        <v>88</v>
       </c>
       <c r="D43" s="1">
-        <v>1.5</v>
+        <v>0.5</v>
       </c>
       <c r="E43" s="1">
-        <v>1.5</v>
+        <v>0.2</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H43" s="22"/>
-      <c r="I43" s="22"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="28" t="s">
-        <v>90</v>
+      <c r="H43" s="22">
+        <f t="shared" si="2"/>
+        <v>0.3</v>
+      </c>
+      <c r="I43" s="22">
+        <f t="shared" si="3"/>
+        <v>149.99999999999997</v>
+      </c>
+    </row>
+    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A44" t="s">
+        <v>89</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>46</v>
+        <v>36</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>37</v>
+        <v>59</v>
       </c>
       <c r="D44" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="E44" s="1">
-        <v>2</v>
+        <v>1.5</v>
       </c>
       <c r="F44" s="4" t="s">
         <v>38</v>
@@ -2108,84 +1906,78 @@
       <c r="H44" s="22"/>
       <c r="I44" s="22"/>
     </row>
-    <row r="45">
-      <c r="A45" s="28" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A45" t="s">
+        <v>90</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D45" s="1">
+        <v>2</v>
+      </c>
+      <c r="E45" s="1">
+        <v>2</v>
+      </c>
+      <c r="F45" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22"/>
+    </row>
+    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A46" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="1" t="s">
+      <c r="B46" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="C45" s="1" t="s">
+      <c r="C46" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="D45" s="1">
+      <c r="D46" s="1">
         <v>3</v>
       </c>
-      <c r="E45" s="1">
+      <c r="E46" s="1">
         <v>3</v>
       </c>
-      <c r="F45" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H45" s="22">
+      <c r="F46" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H46" s="22">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I45" s="22">
+      <c r="I46" s="22">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
     </row>
-    <row r="46">
-      <c r="A46" s="17" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A47" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="B46" s="18"/>
-      <c r="C46" s="19"/>
-      <c r="D46" s="19"/>
-      <c r="E46" s="19"/>
-      <c r="F46" s="21"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I46" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="47">
-      <c r="A47" t="s">
+      <c r="B47" s="18"/>
+      <c r="C47" s="19"/>
+      <c r="D47" s="19"/>
+      <c r="E47" s="19"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="18"/>
+      <c r="H47" s="22" t="str">
+        <f t="shared" si="2"/>
+        <v/>
+      </c>
+      <c r="I47" s="22" t="str">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A48" t="s">
         <v>94</v>
-      </c>
-      <c r="B47" t="s">
-        <v>46</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D47" s="1">
-        <v>4</v>
-      </c>
-      <c r="E47" s="1">
-        <v>6</v>
-      </c>
-      <c r="F47" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="H47" s="22">
-        <f t="shared" si="2"/>
-        <v>-2</v>
-      </c>
-      <c r="I47" s="22">
-        <f t="shared" si="3"/>
-        <v>33.333333333333329</v>
-      </c>
-    </row>
-    <row r="48">
-      <c r="A48" t="s">
-        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
@@ -2194,72 +1986,123 @@
         <v>88</v>
       </c>
       <c r="D48" s="1">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="E48" s="1">
-        <v>0.5</v>
+        <v>6</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>38</v>
+        <v>67</v>
       </c>
       <c r="H48" s="22">
         <f t="shared" si="2"/>
-        <v>0.5</v>
+        <v>-2</v>
       </c>
       <c r="I48" s="22">
         <f t="shared" si="3"/>
-        <v>100</v>
-      </c>
-    </row>
-    <row r="49">
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
       <c r="A49" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B49" t="s">
         <v>46</v>
       </c>
-      <c r="C49" s="29" t="s">
+      <c r="C49" s="1" t="s">
         <v>88</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
       </c>
       <c r="E49" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="F49" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H49" s="22">
+        <f t="shared" si="2"/>
+        <v>0.5</v>
+      </c>
+      <c r="I49" s="22">
+        <f t="shared" si="3"/>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A50" t="s">
+        <v>96</v>
+      </c>
+      <c r="B50" t="s">
+        <v>46</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="D50" s="1">
+        <v>1</v>
+      </c>
+      <c r="E50" s="1">
         <v>0.75</v>
       </c>
-      <c r="F49" s="30" t="s">
+      <c r="F50" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="H49" s="22">
+      <c r="H50" s="22">
         <f t="shared" si="2"/>
         <v>0.25</v>
       </c>
-      <c r="I49" s="22">
+      <c r="I50" s="22">
         <f t="shared" si="3"/>
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="50">
-      <c r="H50" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I50" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="51">
-      <c r="H51" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I51" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="52">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A51" s="28" t="s">
+        <v>97</v>
+      </c>
+      <c r="B51" t="s">
+        <v>46</v>
+      </c>
+      <c r="C51" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D51" s="1">
+        <v>1</v>
+      </c>
+      <c r="E51" s="1">
+        <v>1</v>
+      </c>
+      <c r="F51" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="H51" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I51" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+      <c r="A52" s="28" t="s">
+        <v>99</v>
+      </c>
+      <c r="B52" t="s">
+        <v>46</v>
+      </c>
+      <c r="C52" s="29" t="s">
+        <v>37</v>
+      </c>
+      <c r="D52" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="F52" s="4" t="s">
+        <v>67</v>
+      </c>
       <c r="H52" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2269,7 +2112,7 @@
         <v/>
       </c>
     </row>
-    <row r="53">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H53" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2279,7 +2122,7 @@
         <v/>
       </c>
     </row>
-    <row r="54">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H54" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2289,7 +2132,7 @@
         <v/>
       </c>
     </row>
-    <row r="55">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H55" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2299,7 +2142,7 @@
         <v/>
       </c>
     </row>
-    <row r="56">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H56" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2309,7 +2152,7 @@
         <v/>
       </c>
     </row>
-    <row r="57">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H57" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2319,7 +2162,7 @@
         <v/>
       </c>
     </row>
-    <row r="58">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H58" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2329,7 +2172,7 @@
         <v/>
       </c>
     </row>
-    <row r="59">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H59" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2339,7 +2182,7 @@
         <v/>
       </c>
     </row>
-    <row r="60">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H60" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2349,7 +2192,7 @@
         <v/>
       </c>
     </row>
-    <row r="61">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H61" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2359,7 +2202,7 @@
         <v/>
       </c>
     </row>
-    <row r="62">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H62" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2369,7 +2212,7 @@
         <v/>
       </c>
     </row>
-    <row r="63">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H63" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2379,7 +2222,7 @@
         <v/>
       </c>
     </row>
-    <row r="64">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
       <c r="H64" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2389,7 +2232,7 @@
         <v/>
       </c>
     </row>
-    <row r="65">
+    <row r="65" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H65" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2399,7 +2242,7 @@
         <v/>
       </c>
     </row>
-    <row r="66">
+    <row r="66" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H66" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2409,7 +2252,7 @@
         <v/>
       </c>
     </row>
-    <row r="67">
+    <row r="67" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H67" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2419,7 +2262,7 @@
         <v/>
       </c>
     </row>
-    <row r="68">
+    <row r="68" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H68" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2429,7 +2272,7 @@
         <v/>
       </c>
     </row>
-    <row r="69">
+    <row r="69" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H69" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2439,7 +2282,7 @@
         <v/>
       </c>
     </row>
-    <row r="70">
+    <row r="70" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H70" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2449,7 +2292,7 @@
         <v/>
       </c>
     </row>
-    <row r="71">
+    <row r="71" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H71" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2459,7 +2302,7 @@
         <v/>
       </c>
     </row>
-    <row r="72">
+    <row r="72" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H72" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2469,7 +2312,7 @@
         <v/>
       </c>
     </row>
-    <row r="73">
+    <row r="73" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H73" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2479,27 +2322,27 @@
         <v/>
       </c>
     </row>
-    <row r="74">
+    <row r="74" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H74" s="22" t="str">
-        <f t="shared" ref="H74:H101" si="4">IF(OR(D74="",E74=""),"",D74-E74)</f>
+        <f t="shared" si="2"/>
         <v/>
       </c>
       <c r="I74" s="22" t="str">
-        <f t="shared" ref="I74:I101" si="5">IF(OR(H74="",E74=0),"",ABS(H74)/E74*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="75">
+        <f t="shared" si="3"/>
+        <v/>
+      </c>
+    </row>
+    <row r="75" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H75" s="22" t="str">
-        <f t="shared" si="4"/>
+        <f t="shared" ref="H75:H102" si="4">IF(OR(D75="",E75=""),"",D75-E75)</f>
         <v/>
       </c>
       <c r="I75" s="22" t="str">
-        <f t="shared" si="5"/>
-        <v/>
-      </c>
-    </row>
-    <row r="76">
+        <f t="shared" ref="I75:I102" si="5">IF(OR(H75="",E75=0),"",ABS(H75)/E75*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="76" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H76" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2509,7 +2352,7 @@
         <v/>
       </c>
     </row>
-    <row r="77">
+    <row r="77" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H77" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2519,7 +2362,7 @@
         <v/>
       </c>
     </row>
-    <row r="78">
+    <row r="78" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H78" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2529,7 +2372,7 @@
         <v/>
       </c>
     </row>
-    <row r="79">
+    <row r="79" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H79" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2539,7 +2382,7 @@
         <v/>
       </c>
     </row>
-    <row r="80">
+    <row r="80" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H80" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2549,7 +2392,7 @@
         <v/>
       </c>
     </row>
-    <row r="81">
+    <row r="81" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H81" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2559,7 +2402,7 @@
         <v/>
       </c>
     </row>
-    <row r="82">
+    <row r="82" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H82" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2569,7 +2412,7 @@
         <v/>
       </c>
     </row>
-    <row r="83">
+    <row r="83" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H83" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2579,7 +2422,7 @@
         <v/>
       </c>
     </row>
-    <row r="84">
+    <row r="84" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H84" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2589,7 +2432,7 @@
         <v/>
       </c>
     </row>
-    <row r="85">
+    <row r="85" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H85" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2599,7 +2442,7 @@
         <v/>
       </c>
     </row>
-    <row r="86">
+    <row r="86" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H86" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2609,7 +2452,7 @@
         <v/>
       </c>
     </row>
-    <row r="87">
+    <row r="87" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H87" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2619,7 +2462,7 @@
         <v/>
       </c>
     </row>
-    <row r="88">
+    <row r="88" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H88" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2629,7 +2472,7 @@
         <v/>
       </c>
     </row>
-    <row r="89">
+    <row r="89" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H89" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2639,7 +2482,7 @@
         <v/>
       </c>
     </row>
-    <row r="90">
+    <row r="90" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H90" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2649,7 +2492,7 @@
         <v/>
       </c>
     </row>
-    <row r="91">
+    <row r="91" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H91" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2659,7 +2502,7 @@
         <v/>
       </c>
     </row>
-    <row r="92">
+    <row r="92" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H92" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2669,7 +2512,7 @@
         <v/>
       </c>
     </row>
-    <row r="93">
+    <row r="93" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H93" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2679,7 +2522,7 @@
         <v/>
       </c>
     </row>
-    <row r="94">
+    <row r="94" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H94" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2689,7 +2532,7 @@
         <v/>
       </c>
     </row>
-    <row r="95">
+    <row r="95" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H95" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2699,7 +2542,7 @@
         <v/>
       </c>
     </row>
-    <row r="96">
+    <row r="96" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H96" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2709,7 +2552,7 @@
         <v/>
       </c>
     </row>
-    <row r="97">
+    <row r="97" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H97" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2719,7 +2562,7 @@
         <v/>
       </c>
     </row>
-    <row r="98">
+    <row r="98" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H98" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2729,7 +2572,7 @@
         <v/>
       </c>
     </row>
-    <row r="99">
+    <row r="99" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H99" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2739,7 +2582,7 @@
         <v/>
       </c>
     </row>
-    <row r="100">
+    <row r="100" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H100" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2749,7 +2592,7 @@
         <v/>
       </c>
     </row>
-    <row r="101">
+    <row r="101" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H101" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2759,27 +2602,27 @@
         <v/>
       </c>
     </row>
-    <row r="102">
+    <row r="102" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H102" s="22" t="str">
-        <f t="shared" ref="H102:H165" si="6">IF(OR(D102="",E102=""),"",D102-E102)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I102" s="22" t="str">
-        <f t="shared" ref="I102:I165" si="7">IF(OR(H102="",E102=0),"",ABS(H102)/E102*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="103">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="103" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H103" s="22" t="str">
-        <f t="shared" si="6"/>
+        <f t="shared" ref="H103:H166" si="6">IF(OR(D103="",E103=""),"",D103-E103)</f>
         <v/>
       </c>
       <c r="I103" s="22" t="str">
-        <f t="shared" si="7"/>
-        <v/>
-      </c>
-    </row>
-    <row r="104">
+        <f t="shared" ref="I103:I166" si="7">IF(OR(H103="",E103=0),"",ABS(H103)/E103*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="104" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H104" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2789,7 +2632,7 @@
         <v/>
       </c>
     </row>
-    <row r="105">
+    <row r="105" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H105" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2799,7 +2642,7 @@
         <v/>
       </c>
     </row>
-    <row r="106">
+    <row r="106" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H106" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2809,7 +2652,7 @@
         <v/>
       </c>
     </row>
-    <row r="107">
+    <row r="107" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H107" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2819,7 +2662,7 @@
         <v/>
       </c>
     </row>
-    <row r="108">
+    <row r="108" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H108" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2829,7 +2672,7 @@
         <v/>
       </c>
     </row>
-    <row r="109">
+    <row r="109" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H109" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2839,7 +2682,7 @@
         <v/>
       </c>
     </row>
-    <row r="110">
+    <row r="110" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H110" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2849,7 +2692,7 @@
         <v/>
       </c>
     </row>
-    <row r="111">
+    <row r="111" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H111" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2859,7 +2702,7 @@
         <v/>
       </c>
     </row>
-    <row r="112">
+    <row r="112" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H112" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2869,7 +2712,7 @@
         <v/>
       </c>
     </row>
-    <row r="113">
+    <row r="113" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H113" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2879,7 +2722,7 @@
         <v/>
       </c>
     </row>
-    <row r="114">
+    <row r="114" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H114" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2889,7 +2732,7 @@
         <v/>
       </c>
     </row>
-    <row r="115">
+    <row r="115" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H115" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2899,7 +2742,7 @@
         <v/>
       </c>
     </row>
-    <row r="116">
+    <row r="116" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H116" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2909,7 +2752,7 @@
         <v/>
       </c>
     </row>
-    <row r="117">
+    <row r="117" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H117" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2919,7 +2762,7 @@
         <v/>
       </c>
     </row>
-    <row r="118">
+    <row r="118" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H118" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2929,7 +2772,7 @@
         <v/>
       </c>
     </row>
-    <row r="119">
+    <row r="119" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H119" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2939,7 +2782,7 @@
         <v/>
       </c>
     </row>
-    <row r="120">
+    <row r="120" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H120" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2949,7 +2792,7 @@
         <v/>
       </c>
     </row>
-    <row r="121">
+    <row r="121" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H121" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2959,7 +2802,7 @@
         <v/>
       </c>
     </row>
-    <row r="122">
+    <row r="122" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H122" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2969,7 +2812,7 @@
         <v/>
       </c>
     </row>
-    <row r="123">
+    <row r="123" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H123" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2979,7 +2822,7 @@
         <v/>
       </c>
     </row>
-    <row r="124">
+    <row r="124" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H124" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2989,7 +2832,7 @@
         <v/>
       </c>
     </row>
-    <row r="125">
+    <row r="125" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H125" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2999,7 +2842,7 @@
         <v/>
       </c>
     </row>
-    <row r="126">
+    <row r="126" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H126" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3009,7 +2852,7 @@
         <v/>
       </c>
     </row>
-    <row r="127">
+    <row r="127" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H127" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3019,7 +2862,7 @@
         <v/>
       </c>
     </row>
-    <row r="128">
+    <row r="128" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H128" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3029,7 +2872,7 @@
         <v/>
       </c>
     </row>
-    <row r="129">
+    <row r="129" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H129" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3039,7 +2882,7 @@
         <v/>
       </c>
     </row>
-    <row r="130">
+    <row r="130" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H130" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3049,7 +2892,7 @@
         <v/>
       </c>
     </row>
-    <row r="131">
+    <row r="131" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H131" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3059,7 +2902,7 @@
         <v/>
       </c>
     </row>
-    <row r="132">
+    <row r="132" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H132" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3069,7 +2912,7 @@
         <v/>
       </c>
     </row>
-    <row r="133">
+    <row r="133" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H133" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3079,7 +2922,7 @@
         <v/>
       </c>
     </row>
-    <row r="134">
+    <row r="134" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H134" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3089,7 +2932,7 @@
         <v/>
       </c>
     </row>
-    <row r="135">
+    <row r="135" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H135" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3099,7 +2942,7 @@
         <v/>
       </c>
     </row>
-    <row r="136">
+    <row r="136" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H136" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3109,7 +2952,7 @@
         <v/>
       </c>
     </row>
-    <row r="137">
+    <row r="137" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H137" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3119,7 +2962,7 @@
         <v/>
       </c>
     </row>
-    <row r="138">
+    <row r="138" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H138" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3129,7 +2972,7 @@
         <v/>
       </c>
     </row>
-    <row r="139">
+    <row r="139" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H139" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3139,7 +2982,7 @@
         <v/>
       </c>
     </row>
-    <row r="140">
+    <row r="140" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H140" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3149,7 +2992,7 @@
         <v/>
       </c>
     </row>
-    <row r="141">
+    <row r="141" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H141" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3159,7 +3002,7 @@
         <v/>
       </c>
     </row>
-    <row r="142">
+    <row r="142" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H142" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3169,7 +3012,7 @@
         <v/>
       </c>
     </row>
-    <row r="143">
+    <row r="143" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H143" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3179,7 +3022,7 @@
         <v/>
       </c>
     </row>
-    <row r="144">
+    <row r="144" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H144" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3189,7 +3032,7 @@
         <v/>
       </c>
     </row>
-    <row r="145">
+    <row r="145" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H145" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3199,7 +3042,7 @@
         <v/>
       </c>
     </row>
-    <row r="146">
+    <row r="146" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H146" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3209,7 +3052,7 @@
         <v/>
       </c>
     </row>
-    <row r="147">
+    <row r="147" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H147" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3219,7 +3062,7 @@
         <v/>
       </c>
     </row>
-    <row r="148">
+    <row r="148" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H148" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3229,7 +3072,7 @@
         <v/>
       </c>
     </row>
-    <row r="149">
+    <row r="149" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H149" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3239,7 +3082,7 @@
         <v/>
       </c>
     </row>
-    <row r="150">
+    <row r="150" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H150" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3249,7 +3092,7 @@
         <v/>
       </c>
     </row>
-    <row r="151">
+    <row r="151" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H151" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3259,7 +3102,7 @@
         <v/>
       </c>
     </row>
-    <row r="152">
+    <row r="152" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H152" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3269,7 +3112,7 @@
         <v/>
       </c>
     </row>
-    <row r="153">
+    <row r="153" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H153" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3279,7 +3122,7 @@
         <v/>
       </c>
     </row>
-    <row r="154">
+    <row r="154" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H154" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3289,7 +3132,7 @@
         <v/>
       </c>
     </row>
-    <row r="155">
+    <row r="155" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H155" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3299,7 +3142,7 @@
         <v/>
       </c>
     </row>
-    <row r="156">
+    <row r="156" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H156" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3309,7 +3152,7 @@
         <v/>
       </c>
     </row>
-    <row r="157">
+    <row r="157" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H157" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3319,7 +3162,7 @@
         <v/>
       </c>
     </row>
-    <row r="158">
+    <row r="158" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H158" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3329,7 +3172,7 @@
         <v/>
       </c>
     </row>
-    <row r="159">
+    <row r="159" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H159" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3339,7 +3182,7 @@
         <v/>
       </c>
     </row>
-    <row r="160">
+    <row r="160" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H160" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3349,7 +3192,7 @@
         <v/>
       </c>
     </row>
-    <row r="161">
+    <row r="161" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H161" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3359,7 +3202,7 @@
         <v/>
       </c>
     </row>
-    <row r="162">
+    <row r="162" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H162" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3369,7 +3212,7 @@
         <v/>
       </c>
     </row>
-    <row r="163">
+    <row r="163" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H163" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3379,7 +3222,7 @@
         <v/>
       </c>
     </row>
-    <row r="164">
+    <row r="164" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H164" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3389,7 +3232,7 @@
         <v/>
       </c>
     </row>
-    <row r="165">
+    <row r="165" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H165" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3399,27 +3242,27 @@
         <v/>
       </c>
     </row>
-    <row r="166">
+    <row r="166" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H166" s="22" t="str">
-        <f t="shared" ref="H166:H229" si="8">IF(OR(D166="",E166=""),"",D166-E166)</f>
+        <f t="shared" si="6"/>
         <v/>
       </c>
       <c r="I166" s="22" t="str">
-        <f t="shared" ref="I166:I229" si="9">IF(OR(H166="",E166=0),"",ABS(H166)/E166*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="167">
+        <f t="shared" si="7"/>
+        <v/>
+      </c>
+    </row>
+    <row r="167" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H167" s="22" t="str">
-        <f t="shared" si="8"/>
+        <f t="shared" ref="H167:H230" si="8">IF(OR(D167="",E167=""),"",D167-E167)</f>
         <v/>
       </c>
       <c r="I167" s="22" t="str">
-        <f t="shared" si="9"/>
-        <v/>
-      </c>
-    </row>
-    <row r="168">
+        <f t="shared" ref="I167:I230" si="9">IF(OR(H167="",E167=0),"",ABS(H167)/E167*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="168" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H168" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3429,7 +3272,7 @@
         <v/>
       </c>
     </row>
-    <row r="169">
+    <row r="169" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H169" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3439,7 +3282,7 @@
         <v/>
       </c>
     </row>
-    <row r="170">
+    <row r="170" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H170" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3449,7 +3292,7 @@
         <v/>
       </c>
     </row>
-    <row r="171">
+    <row r="171" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H171" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3459,7 +3302,7 @@
         <v/>
       </c>
     </row>
-    <row r="172">
+    <row r="172" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H172" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3469,7 +3312,7 @@
         <v/>
       </c>
     </row>
-    <row r="173">
+    <row r="173" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H173" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3479,7 +3322,7 @@
         <v/>
       </c>
     </row>
-    <row r="174">
+    <row r="174" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H174" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3489,7 +3332,7 @@
         <v/>
       </c>
     </row>
-    <row r="175">
+    <row r="175" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H175" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3499,7 +3342,7 @@
         <v/>
       </c>
     </row>
-    <row r="176">
+    <row r="176" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H176" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3509,7 +3352,7 @@
         <v/>
       </c>
     </row>
-    <row r="177">
+    <row r="177" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H177" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3519,7 +3362,7 @@
         <v/>
       </c>
     </row>
-    <row r="178">
+    <row r="178" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H178" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3529,7 +3372,7 @@
         <v/>
       </c>
     </row>
-    <row r="179">
+    <row r="179" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H179" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3539,7 +3382,7 @@
         <v/>
       </c>
     </row>
-    <row r="180">
+    <row r="180" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H180" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3549,7 +3392,7 @@
         <v/>
       </c>
     </row>
-    <row r="181">
+    <row r="181" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H181" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3559,7 +3402,7 @@
         <v/>
       </c>
     </row>
-    <row r="182">
+    <row r="182" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H182" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3569,7 +3412,7 @@
         <v/>
       </c>
     </row>
-    <row r="183">
+    <row r="183" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H183" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3579,7 +3422,7 @@
         <v/>
       </c>
     </row>
-    <row r="184">
+    <row r="184" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H184" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3589,7 +3432,7 @@
         <v/>
       </c>
     </row>
-    <row r="185">
+    <row r="185" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H185" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3599,7 +3442,7 @@
         <v/>
       </c>
     </row>
-    <row r="186">
+    <row r="186" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H186" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3609,7 +3452,7 @@
         <v/>
       </c>
     </row>
-    <row r="187">
+    <row r="187" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H187" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3619,7 +3462,7 @@
         <v/>
       </c>
     </row>
-    <row r="188">
+    <row r="188" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H188" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3629,7 +3472,7 @@
         <v/>
       </c>
     </row>
-    <row r="189">
+    <row r="189" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H189" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3639,7 +3482,7 @@
         <v/>
       </c>
     </row>
-    <row r="190">
+    <row r="190" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H190" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3649,7 +3492,7 @@
         <v/>
       </c>
     </row>
-    <row r="191">
+    <row r="191" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H191" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3659,7 +3502,7 @@
         <v/>
       </c>
     </row>
-    <row r="192">
+    <row r="192" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H192" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3669,7 +3512,7 @@
         <v/>
       </c>
     </row>
-    <row r="193">
+    <row r="193" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H193" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3679,7 +3522,7 @@
         <v/>
       </c>
     </row>
-    <row r="194">
+    <row r="194" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H194" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3689,7 +3532,7 @@
         <v/>
       </c>
     </row>
-    <row r="195">
+    <row r="195" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H195" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3699,7 +3542,7 @@
         <v/>
       </c>
     </row>
-    <row r="196">
+    <row r="196" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H196" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3709,7 +3552,7 @@
         <v/>
       </c>
     </row>
-    <row r="197">
+    <row r="197" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H197" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3719,7 +3562,7 @@
         <v/>
       </c>
     </row>
-    <row r="198">
+    <row r="198" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H198" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3729,7 +3572,7 @@
         <v/>
       </c>
     </row>
-    <row r="199">
+    <row r="199" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H199" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3739,7 +3582,7 @@
         <v/>
       </c>
     </row>
-    <row r="200">
+    <row r="200" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H200" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3749,7 +3592,7 @@
         <v/>
       </c>
     </row>
-    <row r="201">
+    <row r="201" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H201" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3759,7 +3602,7 @@
         <v/>
       </c>
     </row>
-    <row r="202">
+    <row r="202" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H202" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3769,7 +3612,7 @@
         <v/>
       </c>
     </row>
-    <row r="203">
+    <row r="203" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H203" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3779,7 +3622,7 @@
         <v/>
       </c>
     </row>
-    <row r="204">
+    <row r="204" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H204" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3789,7 +3632,7 @@
         <v/>
       </c>
     </row>
-    <row r="205">
+    <row r="205" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H205" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3799,7 +3642,7 @@
         <v/>
       </c>
     </row>
-    <row r="206">
+    <row r="206" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H206" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3809,7 +3652,7 @@
         <v/>
       </c>
     </row>
-    <row r="207">
+    <row r="207" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H207" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3819,7 +3662,7 @@
         <v/>
       </c>
     </row>
-    <row r="208">
+    <row r="208" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H208" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3829,7 +3672,7 @@
         <v/>
       </c>
     </row>
-    <row r="209">
+    <row r="209" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H209" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3839,7 +3682,7 @@
         <v/>
       </c>
     </row>
-    <row r="210">
+    <row r="210" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H210" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3849,7 +3692,7 @@
         <v/>
       </c>
     </row>
-    <row r="211">
+    <row r="211" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H211" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3859,7 +3702,7 @@
         <v/>
       </c>
     </row>
-    <row r="212">
+    <row r="212" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H212" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3869,7 +3712,7 @@
         <v/>
       </c>
     </row>
-    <row r="213">
+    <row r="213" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H213" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3879,7 +3722,7 @@
         <v/>
       </c>
     </row>
-    <row r="214">
+    <row r="214" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H214" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3889,7 +3732,7 @@
         <v/>
       </c>
     </row>
-    <row r="215">
+    <row r="215" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H215" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3899,7 +3742,7 @@
         <v/>
       </c>
     </row>
-    <row r="216">
+    <row r="216" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H216" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3909,7 +3752,7 @@
         <v/>
       </c>
     </row>
-    <row r="217">
+    <row r="217" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H217" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3919,7 +3762,7 @@
         <v/>
       </c>
     </row>
-    <row r="218">
+    <row r="218" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H218" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3929,7 +3772,7 @@
         <v/>
       </c>
     </row>
-    <row r="219">
+    <row r="219" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H219" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3939,7 +3782,7 @@
         <v/>
       </c>
     </row>
-    <row r="220">
+    <row r="220" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H220" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3949,7 +3792,7 @@
         <v/>
       </c>
     </row>
-    <row r="221">
+    <row r="221" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H221" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3959,7 +3802,7 @@
         <v/>
       </c>
     </row>
-    <row r="222">
+    <row r="222" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H222" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3969,7 +3812,7 @@
         <v/>
       </c>
     </row>
-    <row r="223">
+    <row r="223" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H223" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3979,7 +3822,7 @@
         <v/>
       </c>
     </row>
-    <row r="224">
+    <row r="224" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H224" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3989,7 +3832,7 @@
         <v/>
       </c>
     </row>
-    <row r="225">
+    <row r="225" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H225" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3999,7 +3842,7 @@
         <v/>
       </c>
     </row>
-    <row r="226">
+    <row r="226" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H226" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4009,7 +3852,7 @@
         <v/>
       </c>
     </row>
-    <row r="227">
+    <row r="227" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H227" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4019,7 +3862,7 @@
         <v/>
       </c>
     </row>
-    <row r="228">
+    <row r="228" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H228" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4029,7 +3872,7 @@
         <v/>
       </c>
     </row>
-    <row r="229">
+    <row r="229" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H229" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -4039,27 +3882,27 @@
         <v/>
       </c>
     </row>
-    <row r="230">
+    <row r="230" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H230" s="22" t="str">
-        <f t="shared" ref="H230:H233" si="10">IF(OR(D230="",E230=""),"",D230-E230)</f>
+        <f t="shared" si="8"/>
         <v/>
       </c>
       <c r="I230" s="22" t="str">
-        <f t="shared" ref="I230:I240" si="11">IF(OR(H230="",E230=0),"",ABS(H230)/E230*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="231">
+        <f t="shared" si="9"/>
+        <v/>
+      </c>
+    </row>
+    <row r="231" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H231" s="22" t="str">
-        <f t="shared" si="10"/>
+        <f t="shared" ref="H231:H234" si="10">IF(OR(D231="",E231=""),"",D231-E231)</f>
         <v/>
       </c>
       <c r="I231" s="22" t="str">
-        <f t="shared" si="11"/>
-        <v/>
-      </c>
-    </row>
-    <row r="232">
+        <f t="shared" ref="I231:I241" si="11">IF(OR(H231="",E231=0),"",ABS(H231)/E231*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="232" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H232" s="22" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -4069,7 +3912,7 @@
         <v/>
       </c>
     </row>
-    <row r="233">
+    <row r="233" spans="8:9" x14ac:dyDescent="0.15">
       <c r="H233" s="22" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -4079,136 +3922,88 @@
         <v/>
       </c>
     </row>
-    <row r="234">
+    <row r="234" spans="8:9" x14ac:dyDescent="0.15">
+      <c r="H234" s="22" t="str">
+        <f t="shared" si="10"/>
+        <v/>
+      </c>
       <c r="I234" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="235">
+    <row r="235" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I235" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="236">
+    <row r="236" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I236" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="237">
+    <row r="237" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I237" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="238">
+    <row r="238" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I238" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="239">
+    <row r="239" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I239" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="240">
+    <row r="240" spans="8:9" x14ac:dyDescent="0.15">
       <c r="I240" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
+    <row r="241" spans="9:9" x14ac:dyDescent="0.15">
+      <c r="I241" s="22" t="str">
+        <f t="shared" si="11"/>
+        <v/>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="F5:F40 F42:F65521">
+    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
+      <formula>"Delayed"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
+      <formula>"Done"</formula>
+    </cfRule>
+    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
+      <formula>"Ongoing"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <dataValidations count="2">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F5:F40 F42:F1241" xr:uid="{004C0068-0053-4772-9BC1-008500B300EB}">
+      <formula1>"Planned,Ongoing,Delayed,Done"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B5:B9 B11:B12 B18:B25 B34 B40:B1241" xr:uid="{00F60079-004C-4143-A0AF-009700D80028}">
+      <formula1>"Requirements,Design,Development,Testing,Preparation,Coordination,Documentation,Interfaces,Delivery"</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
-    <hyperlink location="Instructions!A1" ref="A6"/>
+    <hyperlink ref="A6" location="Instructions!A1" display="    See Instructions sheet for usage" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
   </hyperlinks>
-  <printOptions headings="0" gridLines="1"/>
+  <printOptions gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" scale="70" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;LEdit the Header with Your Team ID&amp;C&amp;F&amp;R&amp;D</oddHeader>
   </headerFooter>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
-      <x14:conditionalFormattings>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{003200B5-006B-481F-BD7A-007000D500DA}">
-            <xm:f>"Delayed"</xm:f>
-            <x14:dxf>
-              <font>
-                <b val="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFDD0806"/>
-                  <bgColor rgb="FFDD0806"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F5:F40 F42:F65520</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00F00075-000D-42E6-B430-00F7007200B3}">
-            <xm:f>"Done"</xm:f>
-            <x14:dxf>
-              <font>
-                <b val="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FF006411"/>
-                  <bgColor rgb="FF006411"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F5:F40 F42:F65520</xm:sqref>
-        </x14:conditionalFormatting>
-        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{009000C3-0040-47E9-B89A-00B2002E0052}">
-            <xm:f>"Ongoing"</xm:f>
-            <x14:dxf>
-              <font>
-                <b val="0"/>
-              </font>
-              <fill>
-                <patternFill patternType="solid">
-                  <fgColor rgb="FFFCF305"/>
-                  <bgColor rgb="FFFCF305"/>
-                </patternFill>
-              </fill>
-            </x14:dxf>
-          </x14:cfRule>
-          <xm:sqref>F5:F40 F42:F65520</xm:sqref>
-        </x14:conditionalFormatting>
-      </x14:conditionalFormattings>
-    </ext>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
-        <x14:dataValidation xr:uid="{004C0068-0053-4772-9BC1-008500B300EB}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-          <x14:formula1>
-            <xm:f>"Planned,Ongoing,Delayed,Done"</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>F5:F40 F42:F1240</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation xr:uid="{00F60079-004C-4143-A0AF-009700D80028}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
-          <x14:formula1>
-            <xm:f>"Requirements,Design,Development,Testing,Preparation,Coordination,Documentation,Interfaces,Delivery"</xm:f>
-          </x14:formula1>
-          <x14:formula2>
-            <xm:f>0</xm:f>
-          </x14:formula2>
-          <xm:sqref>B5:B9 B11:B12 B18:B25 B34 B40:B1240</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
admin view ui updated
</commit_message>
<xml_diff>
--- a/docs/StatusTracker.xlsx
+++ b/docs/StatusTracker.xlsx
@@ -1,113 +1,97 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/aryamirani/Desktop/iiit/sem4/dass/project/project-monorepo-team-20/docs/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21A8F3AE-1AFF-544A-A4FC-A850E505325C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="620" windowWidth="38780" windowHeight="23580" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="15" windowWidth="20955" windowHeight="9720" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Instructions" sheetId="1" r:id="rId1"/>
-    <sheet name="Status" sheetId="2" r:id="rId2"/>
+    <sheet name="Instructions" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Status" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr iterateDelta="0.0001"/>
   <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{D0CA8CA8-9F24-4464-BF8E-62219DCF47F9}"/>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="100">
-  <si>
-    <t>Using the Status tracker</t>
-  </si>
-  <si>
-    <t>At the end of each week, update the status of all activities completed during the week</t>
-  </si>
-  <si>
-    <t>The status tracker shown in this worksheet is an example tracker (values filled are during the middle of the week)</t>
-  </si>
-  <si>
-    <t>Fill in hours spent on each activity during the current week</t>
-  </si>
-  <si>
-    <t>If 5 team members each spent an hour, that counts as 5 hours</t>
-  </si>
-  <si>
-    <t>Fill in time for activities not fully completed ("ongoing") as well, then update these values during following weeks</t>
-  </si>
-  <si>
-    <t>During the planning phases, identify the activities to be done during each week</t>
-  </si>
-  <si>
-    <t>If you spend time on an activity not listed in the tracker, add the activity and list actual hours (need not fill in estimated hours if you didn't estimate it up front)</t>
-  </si>
-  <si>
-    <t>For new activities, identify the type of activity - documentation, coordination, estimation etc.</t>
-  </si>
-  <si>
-    <t>At the end of each week, plan ahead for the following week</t>
-  </si>
-  <si>
-    <t>Identify people responsible for each activity</t>
-  </si>
-  <si>
-    <t>Estimate the hours needed for the activity</t>
-  </si>
-  <si>
-    <t>PROJECT NUMBER</t>
-  </si>
-  <si>
-    <t>PROJECT NAME</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="101">
+  <si>
+    <t xml:space="preserve">Using the Status tracker</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the end of each week, update the status of all activities completed during the week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The status tracker shown in this worksheet is an example tracker (values filled are during the middle of the week)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill in hours spent on each activity during the current week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If 5 team members each spent an hour, that counts as 5 hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fill in time for activities not fully completed ("ongoing") as well, then update these values during following weeks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">During the planning phases, identify the activities to be done during each week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">If you spend time on an activity not listed in the tracker, add the activity and list actual hours (need not fill in estimated hours if you didn't estimate it up front)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">For new activities, identify the type of activity - documentation, coordination, estimation etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">At the end of each week, plan ahead for the following week</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Identify people responsible for each activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimate the hours needed for the activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROJECT NUMBER</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PROJECT NAME</t>
   </si>
   <si>
     <t>S-Learn</t>
   </si>
   <si>
-    <t>PROJECT MENTOR (sponsor)</t>
-  </si>
-  <si>
-    <t>Shankar Foundation</t>
-  </si>
-  <si>
-    <t>TEAM MEMBERS</t>
-  </si>
-  <si>
-    <t>Arya Mirani</t>
-  </si>
-  <si>
-    <t>Vaishnavi K</t>
-  </si>
-  <si>
-    <t>Dev Patel</t>
-  </si>
-  <si>
-    <t>Manan Trivedi</t>
-  </si>
-  <si>
-    <t>Vruddhi Shah</t>
+    <t xml:space="preserve">PROJECT MENTOR (sponsor)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Shankar Foundation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">TEAM MEMBERS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Arya Mirani</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vaishnavi K</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dev Patel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Manan Trivedi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Vruddhi Shah</t>
   </si>
   <si>
     <t>Santhosh</t>
   </si>
   <si>
-    <t>Activity Name</t>
+    <t xml:space="preserve">Activity Name</t>
   </si>
   <si>
     <t>Type</t>
@@ -116,10 +100,10 @@
     <t>Responsible</t>
   </si>
   <si>
-    <t>Estimated Team Hours</t>
-  </si>
-  <si>
-    <t>Actual Hours</t>
+    <t xml:space="preserve">Estimated Team Hours</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Actual Hours</t>
   </si>
   <si>
     <t>Status</t>
@@ -128,19 +112,19 @@
     <t>Comments</t>
   </si>
   <si>
-    <t>Estimation error</t>
-  </si>
-  <si>
-    <t>Estimation error %</t>
+    <t xml:space="preserve">Estimation error</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Estimation error %</t>
   </si>
   <si>
     <t xml:space="preserve">    See Instructions sheet for usage</t>
   </si>
   <si>
-    <t>Week 1 (January 16-  January 17)</t>
-  </si>
-  <si>
-    <t>[Jan 16] Set a meeting with the client</t>
+    <t xml:space="preserve">Week 1 (January 16-  January 17)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Jan 16] Set a meeting with the client</t>
   </si>
   <si>
     <t>Coordination</t>
@@ -152,10 +136,10 @@
     <t>Done</t>
   </si>
   <si>
-    <t>onboarding of the team with the client and knowing the process</t>
-  </si>
-  <si>
-    <t>[Jan 16] Updated design requirements after client meeting</t>
+    <t xml:space="preserve">onboarding of the team with the client and knowing the process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Jan 16] Updated design requirements after client meeting</t>
   </si>
   <si>
     <t>Documentation</t>
@@ -164,28 +148,28 @@
     <t>vaishnavi</t>
   </si>
   <si>
-    <t>update the design requirements according to client feedback, and divide work among team members</t>
-  </si>
-  <si>
-    <t>Week 2 (January 18 - January  24)</t>
-  </si>
-  <si>
-    <t>[jan 18] restructure repository</t>
+    <t xml:space="preserve">update the design requirements according to client feedback, and divide work among team members</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 2 (January 18 - January  24)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[jan 18] restructure repository</t>
   </si>
   <si>
     <t>Development</t>
   </si>
   <si>
-    <t>setup branches and connect to vercel</t>
-  </si>
-  <si>
-    <t>[jan 18] changes requested by client in meeting</t>
-  </si>
-  <si>
-    <t>UI changes</t>
-  </si>
-  <si>
-    <t>[jan 19] changes requested by client in meeting</t>
+    <t xml:space="preserve">setup branches and connect to vercel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[jan 18] changes requested by client in meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[jan 19] changes requested by client in meeting</t>
   </si>
   <si>
     <t>manan</t>
@@ -197,106 +181,109 @@
     <t>vruddhi</t>
   </si>
   <si>
-    <t>[jan 21] restructer the sidebar, other ui improvements</t>
+    <t xml:space="preserve">[jan 21] restructer the sidebar, other ui improvements</t>
   </si>
   <si>
     <t>dev</t>
   </si>
   <si>
-    <t>[Jan 22] client requested changes – color changes, navigation changes between vocabulary exercises</t>
-  </si>
-  <si>
-    <t>[jan 23] Pushed the code to vercel for sending to clients, made website responsive for phone and tablet</t>
-  </si>
-  <si>
-    <t>Meeting 2 with client [Jan 23]</t>
+    <t xml:space="preserve">[Jan 22] client requested changes – color changes, navigation changes between vocabulary exercises</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[jan 23] Pushed the code to vercel for sending to clients, made website responsive for phone and tablet</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Meeting 2 with client [Jan 23]</t>
   </si>
   <si>
     <t>all</t>
   </si>
   <si>
-    <t>updated client on changes made; documented feedback to further changes</t>
-  </si>
-  <si>
-    <t>Week 3 (January 25 – January 31)</t>
-  </si>
-  <si>
-    <t>allocated work in implementing further modules</t>
-  </si>
-  <si>
-    <t>dev, vruddhi ,manan, vaishnavi</t>
-  </si>
-  <si>
-    <t>project synopsis</t>
-  </si>
-  <si>
-    <t>Week 4(Feb 1 - Feb 7)</t>
-  </si>
-  <si>
-    <t>[Feb 1]  make backend database using supabase</t>
+    <t xml:space="preserve">updated client on changes made; documented feedback to further changes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 3 (January 25 – January 31)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">allocated work in implementing further modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">dev, vruddhi ,manan, vaishnavi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">project synopsis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 4(Feb 1 - Feb 7)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Feb 1]  make backend database using supabase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Feb 1] created new modules – evs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 2] created new modules – english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">add new modules in English</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 2-3] created new modules (math word problems, english read words), added exercises to evs module</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 3] Team Internal meeting</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Discussed navigation issues and variations in module implementation; resplit tasks to ensure uniformity among modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 3] created new modules - english </t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 3] refactored and organized codebase for vercel and grade-wise navigation</t>
+  </si>
+  <si>
+    <t xml:space="preserve">navigation changes – dashboard</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Go to Shankar Foundation School [Feb 4]</t>
+  </si>
+  <si>
+    <t>All</t>
+  </si>
+  <si>
+    <t xml:space="preserve">visited the school and saw the process of teaching</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 5] main page dropdown menus, navigation between modules</t>
+  </si>
+  <si>
+    <t xml:space="preserve">added dropdown menu  for the grades on the main page  which further nevigates to the menu of specific subject of that grade and which will nevigate to exersices of that subject .</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Further exercise changes in modules – english</t>
+  </si>
+  <si>
+    <t xml:space="preserve">exercise changes in modules – math</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[feb 7] resizing and rearranging evs</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Week 5 (Feb 8 – Feb 14)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Updating project plan, updating status tracker since first meet</t>
   </si>
   <si>
     <t>Ongoing</t>
   </si>
   <si>
-    <t>[Feb 1] created new modules – evs</t>
-  </si>
-  <si>
-    <t>[feb 2] created new modules – english</t>
-  </si>
-  <si>
-    <t>add new modules in English</t>
-  </si>
-  <si>
-    <t>[feb 2-3] created new modules (math word problems, english read words), added exercises to evs module</t>
-  </si>
-  <si>
-    <t>[feb 3] Team Internal meeting</t>
-  </si>
-  <si>
-    <t>Discussed navigation issues and variations in module implementation; resplit tasks to ensure uniformity among modules</t>
-  </si>
-  <si>
-    <t xml:space="preserve">[feb 3] created new modules - english </t>
-  </si>
-  <si>
-    <t>[feb 3] refactored and organized codebase for vercel and grade-wise navigation</t>
-  </si>
-  <si>
-    <t>navigation changes – dashboard</t>
-  </si>
-  <si>
-    <t>Go to Shankar Foundation School [Feb 4]</t>
-  </si>
-  <si>
-    <t>All</t>
-  </si>
-  <si>
-    <t>visited the school and saw the process of teaching</t>
-  </si>
-  <si>
-    <t>[feb 5] main page dropdown menus, navigation between modules</t>
-  </si>
-  <si>
-    <t>added dropdown menu  for the grades on the main page  which further nevigates to the menu of specific subject of that grade and which will nevigate to exersices of that subject .</t>
-  </si>
-  <si>
-    <t>Further exercise changes in modules – english</t>
-  </si>
-  <si>
-    <t>exercise changes in modules – math</t>
-  </si>
-  <si>
-    <t>[feb 7] resizing and rearranging evs</t>
-  </si>
-  <si>
-    <t>Week 5 (Feb 8 – Feb 14)</t>
-  </si>
-  <si>
-    <t>Updating project plan, updating status tracker since first meet</t>
-  </si>
-  <si>
-    <t>[Feb 11] Computer module fixes requested by client</t>
+    <t xml:space="preserve">connect the frontend to the backend</t>
+  </si>
+  <si>
+    <t xml:space="preserve">[Feb 11] Computer module fixes requested by client</t>
   </si>
   <si>
     <t>Dev</t>
@@ -305,97 +292,86 @@
     <t xml:space="preserve">[feb 10] meeting with sachin sir </t>
   </si>
   <si>
-    <t>add pages for login, singup, teachers, parents, etc.</t>
-  </si>
-  <si>
-    <t>check the backend and frontend connection</t>
+    <t xml:space="preserve">add pages for login, singup, teachers, parents, etc.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">check the backend and frontend connection</t>
   </si>
   <si>
     <t>Testing</t>
   </si>
   <si>
-    <t>Week 6 (Feb 15 – Feb 21)</t>
-  </si>
-  <si>
-    <t>UI Improvements for home pages</t>
-  </si>
-  <si>
-    <t>Changed flow of English exercise</t>
-  </si>
-  <si>
-    <t>Audio clips for English words</t>
-  </si>
-  <si>
-    <t>Fixed the overall flow of the entire modules</t>
-  </si>
-  <si>
-    <t>connect the frontend to the backend</t>
+    <t xml:space="preserve">Week 6 (Feb 15 – Feb 21)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI Improvements for home pages</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Changed flow of English exercise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Audio clips for English words</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed the overall flow of the entire modules</t>
   </si>
   <si>
     <t xml:space="preserve">push the new pages (backend + audiio) to vercel, test the workflow </t>
+  </si>
+  <si>
+    <t xml:space="preserve">UI Changes for admin view</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="11" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="9">
     <font>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <color theme="1"/>
       <name val="Arial"/>
     </font>
     <font>
       <u/>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <color rgb="FF0000D4"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="14"/>
+      <sz val="14.000000"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="14.000000"/>
       <color indexed="4"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="14"/>
+      <sz val="14.000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
-      <sz val="12"/>
+      <sz val="12.000000"/>
       <name val="Arial"/>
     </font>
     <font>
       <b/>
       <u/>
-      <sz val="12"/>
+      <sz val="12.000000"/>
       <color rgb="FF0000D4"/>
       <name val="Arial"/>
     </font>
     <font>
-      <sz val="10"/>
+      <sz val="10.000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -432,141 +408,104 @@
   </fills>
   <borders count="1">
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
+      <left style="none"/>
+      <right style="none"/>
+      <top style="none"/>
+      <bottom style="none"/>
+      <diagonal style="none"/>
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf fontId="1" fillId="0" borderId="0" numFmtId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="31">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf fontId="2" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="3" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="4" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="2" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="6" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
+    <xf fontId="7" fillId="4" borderId="0" numFmtId="0" xfId="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="6" fillId="4" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="6" fillId="4" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1"/>
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="3" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="3" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf fontId="5" fillId="2" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf fontId="8" fillId="0" borderId="0" numFmtId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf fontId="0" fillId="5" borderId="0" numFmtId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf fontId="0" fillId="0" borderId="0" numFmtId="49" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="3">
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFCF305"/>
-          <bgColor rgb="FFFCF305"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FF006411"/>
-          <bgColor rgb="FF006411"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFDD0806"/>
-          <bgColor rgb="FFDD0806"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <colors>
-    <mruColors>
-      <color rgb="FF00FA00"/>
-    </mruColors>
-  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -578,8 +517,291 @@
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ ゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Angsana New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ 明朝"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Cordia New"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:p="http://schemas.openxmlformats.org/presentationml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -631,7 +853,7 @@
         <a:cs typeface="Arial"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme>
+    <a:fmtScheme name="">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -745,90 +967,88 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C27"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
     <sheetView topLeftCell="A15" zoomScale="110" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+      <selection activeCell="B30" activeCellId="0" sqref="B30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13"/>
   <cols>
-    <col min="1" max="1" width="88.33203125" customWidth="1"/>
-    <col min="2" max="2" width="50.33203125" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="88.33203125"/>
+    <col customWidth="1" min="2" max="2" width="50.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="1" ht="18">
       <c r="A1" s="1"/>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="18" x14ac:dyDescent="0.2">
+    <row r="2" ht="18">
       <c r="A2" s="1"/>
       <c r="C2" s="2"/>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="4">
       <c r="A4" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="5">
       <c r="A5" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="6">
       <c r="B6" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="7">
       <c r="B7" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="8">
       <c r="A8" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="9">
       <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="11">
       <c r="A11" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="13">
       <c r="A13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="14">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.15">
+    <row r="15">
       <c r="B15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" ht="30.75" customHeight="1">
       <c r="A19" s="2" t="s">
         <v>12</v>
       </c>
@@ -836,7 +1056,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" ht="25.5" customHeight="1">
       <c r="A20" s="2" t="s">
         <v>13</v>
       </c>
@@ -844,7 +1064,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" ht="25.5" customHeight="1">
       <c r="A21" s="2" t="s">
         <v>15</v>
       </c>
@@ -852,7 +1072,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="37.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" ht="37.5" customHeight="1">
       <c r="A22" s="2" t="s">
         <v>17</v>
       </c>
@@ -860,83 +1080,84 @@
         <v>18</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="23" ht="18">
       <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="24" ht="18">
       <c r="B24" s="3" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="25" ht="18">
       <c r="B25" s="3" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="26" ht="18">
       <c r="B26" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="27" spans="1:2" ht="18" x14ac:dyDescent="0.2">
+    <row r="27" ht="18">
       <c r="B27" s="3"/>
     </row>
   </sheetData>
+  <printOptions headings="0" gridLines="0"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.51181102362204689" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:I241"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac">
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="110" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView topLeftCell="A41" zoomScale="110" workbookViewId="0">
+      <selection activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="13" outlineLevelRow="2" x14ac:dyDescent="0.15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="12.75" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="1" width="50.5" customWidth="1"/>
-    <col min="2" max="2" width="47.6640625" customWidth="1"/>
-    <col min="3" max="3" width="41.83203125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="11" style="1" customWidth="1"/>
-    <col min="5" max="5" width="11.33203125" style="1" customWidth="1"/>
-    <col min="6" max="6" width="12.33203125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="48.33203125" customWidth="1"/>
-    <col min="8" max="9" width="11.33203125" style="5" customWidth="1"/>
+    <col customWidth="1" min="1" max="1" width="50.5"/>
+    <col customWidth="1" min="2" max="2" width="47.6640625"/>
+    <col customWidth="1" min="3" max="3" style="1" width="41.83203125"/>
+    <col customWidth="1" min="4" max="4" style="1" width="11"/>
+    <col customWidth="1" min="5" max="5" style="1" width="11.33203125"/>
+    <col customWidth="1" min="6" max="6" style="4" width="12.33203125"/>
+    <col customWidth="1" min="7" max="7" width="48.33203125"/>
+    <col customWidth="1" min="8" max="9" style="5" width="11.33203125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="24.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" ht="24.75" customHeight="1">
       <c r="A1" s="2" t="str">
         <f>(Instructions!A19)</f>
-        <v>PROJECT NUMBER</v>
+        <v xml:space="preserve">PROJECT NUMBER</v>
       </c>
       <c r="B1" s="6">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="25.5" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" ht="25.5" customHeight="1">
       <c r="A2" s="2" t="str">
         <f>(Instructions!A20)</f>
-        <v>PROJECT NAME</v>
+        <v xml:space="preserve">PROJECT NAME</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:9" ht="30.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" ht="30.75" customHeight="1">
       <c r="A3" s="2" t="str">
         <f>(Instructions!A21)</f>
-        <v>PROJECT MENTOR (sponsor)</v>
+        <v xml:space="preserve">PROJECT MENTOR (sponsor)</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="7" customFormat="1" ht="28" x14ac:dyDescent="0.15">
+    <row r="5" s="7" customFormat="1" ht="38.25">
       <c r="A5" s="8" t="s">
         <v>24</v>
       </c>
@@ -965,7 +1186,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:9" s="13" customFormat="1" ht="30.75" customHeight="1" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="6" s="13" customFormat="1" ht="30.75" customHeight="1" outlineLevel="2">
       <c r="A6" s="14" t="s">
         <v>33</v>
       </c>
@@ -976,7 +1197,7 @@
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
     </row>
-    <row r="7" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="7" outlineLevel="2">
       <c r="A7" s="17" t="s">
         <v>34</v>
       </c>
@@ -995,7 +1216,7 @@
         <v/>
       </c>
     </row>
-    <row r="8" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="8" outlineLevel="2">
       <c r="A8" s="23" t="s">
         <v>35</v>
       </c>
@@ -1026,7 +1247,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="9" outlineLevel="2">
       <c r="A9" t="s">
         <v>40</v>
       </c>
@@ -1050,27 +1271,27 @@
       </c>
       <c r="H9" s="22">
         <f t="shared" si="0"/>
-        <v>-5.0000000000000044E-2</v>
+        <v>-0.050000000000000044</v>
       </c>
       <c r="I9" s="22">
         <f t="shared" si="1"/>
         <v>4.7619047619047654</v>
       </c>
     </row>
-    <row r="10" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="10" outlineLevel="2">
       <c r="A10" s="25"/>
       <c r="B10" s="1"/>
       <c r="C10" s="24"/>
       <c r="H10" s="22" t="str">
-        <f t="shared" ref="H10:H74" si="2">IF(OR(D10="",E10=""),"",D10-E10)</f>
+        <f t="shared" ref="H10:H73" si="2">IF(OR(D10="",E10=""),"",D10-E10)</f>
         <v/>
       </c>
       <c r="I10" s="22" t="str">
-        <f t="shared" ref="I10:I74" si="3">IF(OR(H10="",E10=0),"",ABS(H10)/E10*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="11" spans="1:9" s="18" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
+        <f t="shared" ref="I10:I73" si="3">IF(OR(H10="",E10=0),"",ABS(H10)/E10*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="11" s="18" customFormat="1" outlineLevel="2">
       <c r="A11" s="17" t="s">
         <v>44</v>
       </c>
@@ -1087,7 +1308,7 @@
         <v/>
       </c>
     </row>
-    <row r="12" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="12" ht="14" outlineLevel="2">
       <c r="A12" s="25" t="s">
         <v>45</v>
       </c>
@@ -1118,7 +1339,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="18" customFormat="1" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="13" s="18" customFormat="1" ht="14" outlineLevel="2">
       <c r="A13" s="25" t="s">
         <v>48</v>
       </c>
@@ -1149,7 +1370,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="18" customFormat="1" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="14" s="18" customFormat="1" ht="14" outlineLevel="2">
       <c r="A14" s="25" t="s">
         <v>50</v>
       </c>
@@ -1176,7 +1397,7 @@
         <v/>
       </c>
     </row>
-    <row r="15" spans="1:9" s="18" customFormat="1" ht="42" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="15" s="18" customFormat="1" ht="25.5" outlineLevel="2">
       <c r="A15" s="25" t="s">
         <v>52</v>
       </c>
@@ -1207,7 +1428,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="18" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="16" s="18" customFormat="1" ht="28" outlineLevel="2">
       <c r="A16" s="25" t="s">
         <v>54</v>
       </c>
@@ -1234,7 +1455,7 @@
         <v/>
       </c>
     </row>
-    <row r="17" spans="1:9" s="18" customFormat="1" ht="28" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="17" s="18" customFormat="1" ht="25.5" outlineLevel="2">
       <c r="A17" s="25" t="s">
         <v>56</v>
       </c>
@@ -1265,7 +1486,7 @@
         <v>63.636363636363633</v>
       </c>
     </row>
-    <row r="18" spans="1:9" ht="42" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="18" ht="25.5" outlineLevel="2">
       <c r="A18" s="25" t="s">
         <v>57</v>
       </c>
@@ -1293,7 +1514,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="14" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="19" ht="14" outlineLevel="2">
       <c r="A19" s="25" t="s">
         <v>58</v>
       </c>
@@ -1324,7 +1545,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:9" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="20" outlineLevel="2">
       <c r="A20" s="25"/>
       <c r="B20" s="1"/>
       <c r="H20" s="22" t="str">
@@ -1336,7 +1557,7 @@
         <v/>
       </c>
     </row>
-    <row r="21" spans="1:9" s="18" customFormat="1" outlineLevel="2" x14ac:dyDescent="0.15">
+    <row r="21" s="18" customFormat="1" outlineLevel="2">
       <c r="A21" s="17" t="s">
         <v>61</v>
       </c>
@@ -1353,7 +1574,7 @@
         <v/>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="22">
       <c r="A22" t="s">
         <v>62</v>
       </c>
@@ -1381,7 +1602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="23">
       <c r="A23" t="s">
         <v>64</v>
       </c>
@@ -1403,7 +1624,7 @@
         <v/>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="24">
       <c r="H24" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -1413,7 +1634,7 @@
         <v/>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="25">
       <c r="A25" s="17" t="s">
         <v>65</v>
       </c>
@@ -1432,7 +1653,7 @@
         <v/>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="26">
       <c r="A26" s="23" t="s">
         <v>66</v>
       </c>
@@ -1460,9 +1681,9 @@
         <v>9.0909090909090917</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="27">
       <c r="A27" s="23" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>46</v>
@@ -1483,9 +1704,9 @@
         <v/>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="28">
       <c r="A28" s="23" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>46</v>
@@ -1503,20 +1724,20 @@
         <v>38</v>
       </c>
       <c r="G28" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H28" s="22">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="I28" s="22">
+        <f t="shared" si="3"/>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" s="23" t="s">
         <v>70</v>
-      </c>
-      <c r="H28" s="22">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="I28" s="22">
-        <f t="shared" si="3"/>
-        <v>33.333333333333329</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A29" s="30" t="s">
-        <v>71</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>46</v>
@@ -1543,9 +1764,9 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="30">
       <c r="A30" s="23" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>36</v>
@@ -1563,20 +1784,20 @@
         <v>38</v>
       </c>
       <c r="G30" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H30" s="22">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I30" s="22">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" s="23" t="s">
         <v>73</v>
-      </c>
-      <c r="H30" s="22">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="I30" s="22">
-        <f t="shared" si="3"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A31" s="23" t="s">
-        <v>74</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>46</v>
@@ -1597,9 +1818,9 @@
         <v/>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="32">
       <c r="A32" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>46</v>
@@ -1619,9 +1840,9 @@
         <v/>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="33">
       <c r="A33" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>46</v>
@@ -1641,15 +1862,15 @@
         <v/>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="34">
       <c r="A34" s="23" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>36</v>
       </c>
       <c r="C34" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D34" s="1">
         <v>2</v>
@@ -1661,20 +1882,20 @@
         <v>38</v>
       </c>
       <c r="G34" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="H34" s="22">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="I34" s="22">
+        <f t="shared" si="3"/>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="s">
         <v>79</v>
-      </c>
-      <c r="H34" s="22">
-        <f t="shared" si="2"/>
-        <v>-1</v>
-      </c>
-      <c r="I34" s="22">
-        <f t="shared" si="3"/>
-        <v>33.333333333333329</v>
-      </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A35" t="s">
-        <v>80</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>46</v>
@@ -1692,20 +1913,20 @@
         <v>38</v>
       </c>
       <c r="G35" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="H35" s="22">
+        <f t="shared" si="2"/>
+        <v>-0.5</v>
+      </c>
+      <c r="I35" s="22">
+        <f t="shared" si="3"/>
+        <v>33.333333333333329</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="s">
         <v>81</v>
-      </c>
-      <c r="H35" s="22">
-        <f t="shared" si="2"/>
-        <v>-0.5</v>
-      </c>
-      <c r="I35" s="22">
-        <f t="shared" si="3"/>
-        <v>33.333333333333329</v>
-      </c>
-    </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="A36" t="s">
-        <v>82</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>46</v>
@@ -1725,9 +1946,9 @@
         <v/>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="37">
       <c r="A37" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>46</v>
@@ -1753,9 +1974,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="38">
       <c r="A38" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>46</v>
@@ -1775,7 +1996,7 @@
         <v/>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="39">
       <c r="B39" s="1"/>
       <c r="H39" s="22" t="str">
         <f t="shared" si="2"/>
@@ -1786,9 +2007,9 @@
         <v/>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="40">
       <c r="A40" s="17" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B40" s="18"/>
       <c r="C40" s="19"/>
@@ -1805,9 +2026,9 @@
         <v/>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="41">
       <c r="A41" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>41</v>
@@ -1819,7 +2040,7 @@
         <v>3</v>
       </c>
       <c r="F41" s="27" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="H41" s="22" t="str">
         <f t="shared" si="2"/>
@@ -1830,14 +2051,14 @@
         <v/>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="42">
       <c r="A42" s="28" t="s">
-        <v>98</v>
+        <v>87</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="C42" s="29" t="s">
+      <c r="C42" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D42" s="1">
@@ -1856,37 +2077,37 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="43">
       <c r="A43" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>46</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D43" s="1">
         <v>0.5</v>
       </c>
       <c r="E43" s="1">
-        <v>0.2</v>
+        <v>0.20000000000000001</v>
       </c>
       <c r="F43" s="4" t="s">
         <v>38</v>
       </c>
       <c r="H43" s="22">
         <f t="shared" si="2"/>
-        <v>0.3</v>
+        <v>0.29999999999999999</v>
       </c>
       <c r="I43" s="22">
         <f t="shared" si="3"/>
         <v>149.99999999999997</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="44">
       <c r="A44" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>36</v>
@@ -1906,9 +2127,9 @@
       <c r="H44" s="22"/>
       <c r="I44" s="22"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="45">
       <c r="A45" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>46</v>
@@ -1928,12 +2149,12 @@
       <c r="H45" s="22"/>
       <c r="I45" s="22"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="46">
       <c r="A46" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="C46" s="1" t="s">
         <v>59</v>
@@ -1956,9 +2177,9 @@
         <v>0</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="47">
       <c r="A47" s="17" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B47" s="18"/>
       <c r="C47" s="19"/>
@@ -1975,15 +2196,15 @@
         <v/>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="48">
       <c r="A48" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B48" t="s">
         <v>46</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D48" s="1">
         <v>4</v>
@@ -1992,7 +2213,7 @@
         <v>6</v>
       </c>
       <c r="F48" s="4" t="s">
-        <v>67</v>
+        <v>38</v>
       </c>
       <c r="H48" s="22">
         <f t="shared" si="2"/>
@@ -2003,15 +2224,15 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="49">
       <c r="A49" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B49" t="s">
         <v>46</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D49" s="1">
         <v>1</v>
@@ -2031,15 +2252,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="50">
       <c r="A50" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B50" t="s">
         <v>46</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D50" s="1">
         <v>1</v>
@@ -2059,14 +2280,14 @@
         <v>33.333333333333329</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="51">
       <c r="A51" s="28" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B51" t="s">
         <v>46</v>
       </c>
-      <c r="C51" s="29" t="s">
+      <c r="C51" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D51" s="1">
@@ -2087,21 +2308,21 @@
         <v>0</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="52">
       <c r="A52" s="28" t="s">
         <v>99</v>
       </c>
       <c r="B52" t="s">
         <v>46</v>
       </c>
-      <c r="C52" s="29" t="s">
+      <c r="C52" s="1" t="s">
         <v>37</v>
       </c>
       <c r="D52" s="1">
         <v>2.5</v>
       </c>
       <c r="F52" s="4" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="H52" s="22" t="str">
         <f t="shared" si="2"/>
@@ -2112,17 +2333,35 @@
         <v/>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.15">
-      <c r="H53" s="22" t="str">
-        <f t="shared" si="2"/>
-        <v/>
-      </c>
-      <c r="I53" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="53">
+      <c r="A53" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" t="s">
+        <v>46</v>
+      </c>
+      <c r="C53" s="29" t="s">
+        <v>89</v>
+      </c>
+      <c r="D53" s="1">
+        <v>3</v>
+      </c>
+      <c r="E53" s="1">
+        <v>4</v>
+      </c>
+      <c r="F53" s="30" t="s">
+        <v>38</v>
+      </c>
+      <c r="H53" s="22">
+        <f t="shared" si="2"/>
+        <v>-1</v>
+      </c>
+      <c r="I53" s="22">
+        <f t="shared" si="3"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="54">
       <c r="H54" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2132,7 +2371,7 @@
         <v/>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="55">
       <c r="H55" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2142,7 +2381,7 @@
         <v/>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="56">
       <c r="H56" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2152,7 +2391,7 @@
         <v/>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="57">
       <c r="H57" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2162,7 +2401,7 @@
         <v/>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="58">
       <c r="H58" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2172,7 +2411,7 @@
         <v/>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="59">
       <c r="H59" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2182,7 +2421,7 @@
         <v/>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="60">
       <c r="H60" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2192,7 +2431,7 @@
         <v/>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="61">
       <c r="H61" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2202,7 +2441,7 @@
         <v/>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="62">
       <c r="H62" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2212,7 +2451,7 @@
         <v/>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="63">
       <c r="H63" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2222,7 +2461,7 @@
         <v/>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.15">
+    <row r="64">
       <c r="H64" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2232,7 +2471,7 @@
         <v/>
       </c>
     </row>
-    <row r="65" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="65">
       <c r="H65" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2242,7 +2481,7 @@
         <v/>
       </c>
     </row>
-    <row r="66" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="66">
       <c r="H66" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2252,7 +2491,7 @@
         <v/>
       </c>
     </row>
-    <row r="67" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="67">
       <c r="H67" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2262,7 +2501,7 @@
         <v/>
       </c>
     </row>
-    <row r="68" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="68">
       <c r="H68" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2272,7 +2511,7 @@
         <v/>
       </c>
     </row>
-    <row r="69" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="69">
       <c r="H69" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2282,7 +2521,7 @@
         <v/>
       </c>
     </row>
-    <row r="70" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="70">
       <c r="H70" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2292,7 +2531,7 @@
         <v/>
       </c>
     </row>
-    <row r="71" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="71">
       <c r="H71" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2302,7 +2541,7 @@
         <v/>
       </c>
     </row>
-    <row r="72" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="72">
       <c r="H72" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2312,7 +2551,7 @@
         <v/>
       </c>
     </row>
-    <row r="73" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="73">
       <c r="H73" s="22" t="str">
         <f t="shared" si="2"/>
         <v/>
@@ -2322,27 +2561,27 @@
         <v/>
       </c>
     </row>
-    <row r="74" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="74">
       <c r="H74" s="22" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="H74:H102" si="4">IF(OR(D74="",E74=""),"",D74-E74)</f>
         <v/>
       </c>
       <c r="I74" s="22" t="str">
-        <f t="shared" si="3"/>
-        <v/>
-      </c>
-    </row>
-    <row r="75" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" ref="I74:I102" si="5">IF(OR(H74="",E74=0),"",ABS(H74)/E74*100)</f>
+        <v/>
+      </c>
+    </row>
+    <row r="75">
       <c r="H75" s="22" t="str">
-        <f t="shared" ref="H75:H102" si="4">IF(OR(D75="",E75=""),"",D75-E75)</f>
+        <f t="shared" si="4"/>
         <v/>
       </c>
       <c r="I75" s="22" t="str">
-        <f t="shared" ref="I75:I102" si="5">IF(OR(H75="",E75=0),"",ABS(H75)/E75*100)</f>
-        <v/>
-      </c>
-    </row>
-    <row r="76" spans="8:9" x14ac:dyDescent="0.15">
+        <f t="shared" si="5"/>
+        <v/>
+      </c>
+    </row>
+    <row r="76">
       <c r="H76" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2352,7 +2591,7 @@
         <v/>
       </c>
     </row>
-    <row r="77" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="77">
       <c r="H77" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2362,7 +2601,7 @@
         <v/>
       </c>
     </row>
-    <row r="78" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="78">
       <c r="H78" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2372,7 +2611,7 @@
         <v/>
       </c>
     </row>
-    <row r="79" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="79">
       <c r="H79" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2382,7 +2621,7 @@
         <v/>
       </c>
     </row>
-    <row r="80" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="80">
       <c r="H80" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2392,7 +2631,7 @@
         <v/>
       </c>
     </row>
-    <row r="81" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="81">
       <c r="H81" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2402,7 +2641,7 @@
         <v/>
       </c>
     </row>
-    <row r="82" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="82">
       <c r="H82" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2412,7 +2651,7 @@
         <v/>
       </c>
     </row>
-    <row r="83" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="83">
       <c r="H83" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2422,7 +2661,7 @@
         <v/>
       </c>
     </row>
-    <row r="84" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="84">
       <c r="H84" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2432,7 +2671,7 @@
         <v/>
       </c>
     </row>
-    <row r="85" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="85">
       <c r="H85" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2442,7 +2681,7 @@
         <v/>
       </c>
     </row>
-    <row r="86" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="86">
       <c r="H86" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2452,7 +2691,7 @@
         <v/>
       </c>
     </row>
-    <row r="87" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="87">
       <c r="H87" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2462,7 +2701,7 @@
         <v/>
       </c>
     </row>
-    <row r="88" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="88">
       <c r="H88" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2472,7 +2711,7 @@
         <v/>
       </c>
     </row>
-    <row r="89" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="89">
       <c r="H89" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2482,7 +2721,7 @@
         <v/>
       </c>
     </row>
-    <row r="90" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="90">
       <c r="H90" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2492,7 +2731,7 @@
         <v/>
       </c>
     </row>
-    <row r="91" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="91">
       <c r="H91" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2502,7 +2741,7 @@
         <v/>
       </c>
     </row>
-    <row r="92" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="92">
       <c r="H92" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2512,7 +2751,7 @@
         <v/>
       </c>
     </row>
-    <row r="93" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="93">
       <c r="H93" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2522,7 +2761,7 @@
         <v/>
       </c>
     </row>
-    <row r="94" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="94">
       <c r="H94" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2532,7 +2771,7 @@
         <v/>
       </c>
     </row>
-    <row r="95" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="95">
       <c r="H95" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2542,7 +2781,7 @@
         <v/>
       </c>
     </row>
-    <row r="96" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="96">
       <c r="H96" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2552,7 +2791,7 @@
         <v/>
       </c>
     </row>
-    <row r="97" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="97">
       <c r="H97" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2562,7 +2801,7 @@
         <v/>
       </c>
     </row>
-    <row r="98" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="98">
       <c r="H98" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2572,7 +2811,7 @@
         <v/>
       </c>
     </row>
-    <row r="99" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="99">
       <c r="H99" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2582,7 +2821,7 @@
         <v/>
       </c>
     </row>
-    <row r="100" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="100">
       <c r="H100" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2592,7 +2831,7 @@
         <v/>
       </c>
     </row>
-    <row r="101" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="101">
       <c r="H101" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2602,7 +2841,7 @@
         <v/>
       </c>
     </row>
-    <row r="102" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="102">
       <c r="H102" s="22" t="str">
         <f t="shared" si="4"/>
         <v/>
@@ -2612,7 +2851,7 @@
         <v/>
       </c>
     </row>
-    <row r="103" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="103">
       <c r="H103" s="22" t="str">
         <f t="shared" ref="H103:H166" si="6">IF(OR(D103="",E103=""),"",D103-E103)</f>
         <v/>
@@ -2622,7 +2861,7 @@
         <v/>
       </c>
     </row>
-    <row r="104" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="104">
       <c r="H104" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2632,7 +2871,7 @@
         <v/>
       </c>
     </row>
-    <row r="105" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="105">
       <c r="H105" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2642,7 +2881,7 @@
         <v/>
       </c>
     </row>
-    <row r="106" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="106">
       <c r="H106" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2652,7 +2891,7 @@
         <v/>
       </c>
     </row>
-    <row r="107" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="107">
       <c r="H107" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2662,7 +2901,7 @@
         <v/>
       </c>
     </row>
-    <row r="108" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="108">
       <c r="H108" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2672,7 +2911,7 @@
         <v/>
       </c>
     </row>
-    <row r="109" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="109">
       <c r="H109" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2682,7 +2921,7 @@
         <v/>
       </c>
     </row>
-    <row r="110" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="110">
       <c r="H110" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2692,7 +2931,7 @@
         <v/>
       </c>
     </row>
-    <row r="111" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="111">
       <c r="H111" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2702,7 +2941,7 @@
         <v/>
       </c>
     </row>
-    <row r="112" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="112">
       <c r="H112" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2712,7 +2951,7 @@
         <v/>
       </c>
     </row>
-    <row r="113" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="113">
       <c r="H113" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2722,7 +2961,7 @@
         <v/>
       </c>
     </row>
-    <row r="114" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="114">
       <c r="H114" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2732,7 +2971,7 @@
         <v/>
       </c>
     </row>
-    <row r="115" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="115">
       <c r="H115" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2742,7 +2981,7 @@
         <v/>
       </c>
     </row>
-    <row r="116" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="116">
       <c r="H116" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2752,7 +2991,7 @@
         <v/>
       </c>
     </row>
-    <row r="117" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="117">
       <c r="H117" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2762,7 +3001,7 @@
         <v/>
       </c>
     </row>
-    <row r="118" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="118">
       <c r="H118" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2772,7 +3011,7 @@
         <v/>
       </c>
     </row>
-    <row r="119" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="119">
       <c r="H119" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2782,7 +3021,7 @@
         <v/>
       </c>
     </row>
-    <row r="120" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="120">
       <c r="H120" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2792,7 +3031,7 @@
         <v/>
       </c>
     </row>
-    <row r="121" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="121">
       <c r="H121" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2802,7 +3041,7 @@
         <v/>
       </c>
     </row>
-    <row r="122" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="122">
       <c r="H122" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2812,7 +3051,7 @@
         <v/>
       </c>
     </row>
-    <row r="123" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="123">
       <c r="H123" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2822,7 +3061,7 @@
         <v/>
       </c>
     </row>
-    <row r="124" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="124">
       <c r="H124" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2832,7 +3071,7 @@
         <v/>
       </c>
     </row>
-    <row r="125" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="125">
       <c r="H125" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2842,7 +3081,7 @@
         <v/>
       </c>
     </row>
-    <row r="126" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="126">
       <c r="H126" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2852,7 +3091,7 @@
         <v/>
       </c>
     </row>
-    <row r="127" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="127">
       <c r="H127" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2862,7 +3101,7 @@
         <v/>
       </c>
     </row>
-    <row r="128" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="128">
       <c r="H128" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2872,7 +3111,7 @@
         <v/>
       </c>
     </row>
-    <row r="129" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="129">
       <c r="H129" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2882,7 +3121,7 @@
         <v/>
       </c>
     </row>
-    <row r="130" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="130">
       <c r="H130" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2892,7 +3131,7 @@
         <v/>
       </c>
     </row>
-    <row r="131" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="131">
       <c r="H131" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2902,7 +3141,7 @@
         <v/>
       </c>
     </row>
-    <row r="132" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="132">
       <c r="H132" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2912,7 +3151,7 @@
         <v/>
       </c>
     </row>
-    <row r="133" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="133">
       <c r="H133" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2922,7 +3161,7 @@
         <v/>
       </c>
     </row>
-    <row r="134" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="134">
       <c r="H134" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2932,7 +3171,7 @@
         <v/>
       </c>
     </row>
-    <row r="135" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="135">
       <c r="H135" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2942,7 +3181,7 @@
         <v/>
       </c>
     </row>
-    <row r="136" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="136">
       <c r="H136" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2952,7 +3191,7 @@
         <v/>
       </c>
     </row>
-    <row r="137" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="137">
       <c r="H137" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2962,7 +3201,7 @@
         <v/>
       </c>
     </row>
-    <row r="138" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="138">
       <c r="H138" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2972,7 +3211,7 @@
         <v/>
       </c>
     </row>
-    <row r="139" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="139">
       <c r="H139" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2982,7 +3221,7 @@
         <v/>
       </c>
     </row>
-    <row r="140" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="140">
       <c r="H140" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -2992,7 +3231,7 @@
         <v/>
       </c>
     </row>
-    <row r="141" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="141">
       <c r="H141" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3002,7 +3241,7 @@
         <v/>
       </c>
     </row>
-    <row r="142" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="142">
       <c r="H142" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3012,7 +3251,7 @@
         <v/>
       </c>
     </row>
-    <row r="143" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="143">
       <c r="H143" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3022,7 +3261,7 @@
         <v/>
       </c>
     </row>
-    <row r="144" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="144">
       <c r="H144" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3032,7 +3271,7 @@
         <v/>
       </c>
     </row>
-    <row r="145" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="145">
       <c r="H145" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3042,7 +3281,7 @@
         <v/>
       </c>
     </row>
-    <row r="146" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="146">
       <c r="H146" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3052,7 +3291,7 @@
         <v/>
       </c>
     </row>
-    <row r="147" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="147">
       <c r="H147" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3062,7 +3301,7 @@
         <v/>
       </c>
     </row>
-    <row r="148" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="148">
       <c r="H148" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3072,7 +3311,7 @@
         <v/>
       </c>
     </row>
-    <row r="149" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="149">
       <c r="H149" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3082,7 +3321,7 @@
         <v/>
       </c>
     </row>
-    <row r="150" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="150">
       <c r="H150" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3092,7 +3331,7 @@
         <v/>
       </c>
     </row>
-    <row r="151" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="151">
       <c r="H151" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3102,7 +3341,7 @@
         <v/>
       </c>
     </row>
-    <row r="152" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="152">
       <c r="H152" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3112,7 +3351,7 @@
         <v/>
       </c>
     </row>
-    <row r="153" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="153">
       <c r="H153" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3122,7 +3361,7 @@
         <v/>
       </c>
     </row>
-    <row r="154" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="154">
       <c r="H154" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3132,7 +3371,7 @@
         <v/>
       </c>
     </row>
-    <row r="155" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="155">
       <c r="H155" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3142,7 +3381,7 @@
         <v/>
       </c>
     </row>
-    <row r="156" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="156">
       <c r="H156" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3152,7 +3391,7 @@
         <v/>
       </c>
     </row>
-    <row r="157" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="157">
       <c r="H157" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3162,7 +3401,7 @@
         <v/>
       </c>
     </row>
-    <row r="158" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="158">
       <c r="H158" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3172,7 +3411,7 @@
         <v/>
       </c>
     </row>
-    <row r="159" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="159">
       <c r="H159" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3182,7 +3421,7 @@
         <v/>
       </c>
     </row>
-    <row r="160" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="160">
       <c r="H160" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3192,7 +3431,7 @@
         <v/>
       </c>
     </row>
-    <row r="161" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="161">
       <c r="H161" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3202,7 +3441,7 @@
         <v/>
       </c>
     </row>
-    <row r="162" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="162">
       <c r="H162" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3212,7 +3451,7 @@
         <v/>
       </c>
     </row>
-    <row r="163" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="163">
       <c r="H163" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3222,7 +3461,7 @@
         <v/>
       </c>
     </row>
-    <row r="164" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="164">
       <c r="H164" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3232,7 +3471,7 @@
         <v/>
       </c>
     </row>
-    <row r="165" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="165">
       <c r="H165" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3242,7 +3481,7 @@
         <v/>
       </c>
     </row>
-    <row r="166" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="166">
       <c r="H166" s="22" t="str">
         <f t="shared" si="6"/>
         <v/>
@@ -3252,7 +3491,7 @@
         <v/>
       </c>
     </row>
-    <row r="167" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="167">
       <c r="H167" s="22" t="str">
         <f t="shared" ref="H167:H230" si="8">IF(OR(D167="",E167=""),"",D167-E167)</f>
         <v/>
@@ -3262,7 +3501,7 @@
         <v/>
       </c>
     </row>
-    <row r="168" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="168">
       <c r="H168" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3272,7 +3511,7 @@
         <v/>
       </c>
     </row>
-    <row r="169" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="169">
       <c r="H169" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3282,7 +3521,7 @@
         <v/>
       </c>
     </row>
-    <row r="170" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="170">
       <c r="H170" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3292,7 +3531,7 @@
         <v/>
       </c>
     </row>
-    <row r="171" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="171">
       <c r="H171" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3302,7 +3541,7 @@
         <v/>
       </c>
     </row>
-    <row r="172" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="172">
       <c r="H172" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3312,7 +3551,7 @@
         <v/>
       </c>
     </row>
-    <row r="173" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="173">
       <c r="H173" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3322,7 +3561,7 @@
         <v/>
       </c>
     </row>
-    <row r="174" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="174">
       <c r="H174" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3332,7 +3571,7 @@
         <v/>
       </c>
     </row>
-    <row r="175" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="175">
       <c r="H175" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3342,7 +3581,7 @@
         <v/>
       </c>
     </row>
-    <row r="176" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="176">
       <c r="H176" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3352,7 +3591,7 @@
         <v/>
       </c>
     </row>
-    <row r="177" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="177">
       <c r="H177" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3362,7 +3601,7 @@
         <v/>
       </c>
     </row>
-    <row r="178" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="178">
       <c r="H178" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3372,7 +3611,7 @@
         <v/>
       </c>
     </row>
-    <row r="179" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="179">
       <c r="H179" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3382,7 +3621,7 @@
         <v/>
       </c>
     </row>
-    <row r="180" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="180">
       <c r="H180" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3392,7 +3631,7 @@
         <v/>
       </c>
     </row>
-    <row r="181" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="181">
       <c r="H181" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3402,7 +3641,7 @@
         <v/>
       </c>
     </row>
-    <row r="182" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="182">
       <c r="H182" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3412,7 +3651,7 @@
         <v/>
       </c>
     </row>
-    <row r="183" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="183">
       <c r="H183" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3422,7 +3661,7 @@
         <v/>
       </c>
     </row>
-    <row r="184" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="184">
       <c r="H184" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3432,7 +3671,7 @@
         <v/>
       </c>
     </row>
-    <row r="185" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="185">
       <c r="H185" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3442,7 +3681,7 @@
         <v/>
       </c>
     </row>
-    <row r="186" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="186">
       <c r="H186" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3452,7 +3691,7 @@
         <v/>
       </c>
     </row>
-    <row r="187" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="187">
       <c r="H187" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3462,7 +3701,7 @@
         <v/>
       </c>
     </row>
-    <row r="188" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="188">
       <c r="H188" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3472,7 +3711,7 @@
         <v/>
       </c>
     </row>
-    <row r="189" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="189">
       <c r="H189" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3482,7 +3721,7 @@
         <v/>
       </c>
     </row>
-    <row r="190" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="190">
       <c r="H190" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3492,7 +3731,7 @@
         <v/>
       </c>
     </row>
-    <row r="191" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="191">
       <c r="H191" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3502,7 +3741,7 @@
         <v/>
       </c>
     </row>
-    <row r="192" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="192">
       <c r="H192" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3512,7 +3751,7 @@
         <v/>
       </c>
     </row>
-    <row r="193" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="193">
       <c r="H193" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3522,7 +3761,7 @@
         <v/>
       </c>
     </row>
-    <row r="194" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="194">
       <c r="H194" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3532,7 +3771,7 @@
         <v/>
       </c>
     </row>
-    <row r="195" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="195">
       <c r="H195" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3542,7 +3781,7 @@
         <v/>
       </c>
     </row>
-    <row r="196" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="196">
       <c r="H196" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3552,7 +3791,7 @@
         <v/>
       </c>
     </row>
-    <row r="197" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="197">
       <c r="H197" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3562,7 +3801,7 @@
         <v/>
       </c>
     </row>
-    <row r="198" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="198">
       <c r="H198" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3572,7 +3811,7 @@
         <v/>
       </c>
     </row>
-    <row r="199" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="199">
       <c r="H199" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3582,7 +3821,7 @@
         <v/>
       </c>
     </row>
-    <row r="200" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="200">
       <c r="H200" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3592,7 +3831,7 @@
         <v/>
       </c>
     </row>
-    <row r="201" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="201">
       <c r="H201" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3602,7 +3841,7 @@
         <v/>
       </c>
     </row>
-    <row r="202" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="202">
       <c r="H202" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3612,7 +3851,7 @@
         <v/>
       </c>
     </row>
-    <row r="203" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="203">
       <c r="H203" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3622,7 +3861,7 @@
         <v/>
       </c>
     </row>
-    <row r="204" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="204">
       <c r="H204" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3632,7 +3871,7 @@
         <v/>
       </c>
     </row>
-    <row r="205" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="205">
       <c r="H205" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3642,7 +3881,7 @@
         <v/>
       </c>
     </row>
-    <row r="206" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="206">
       <c r="H206" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3652,7 +3891,7 @@
         <v/>
       </c>
     </row>
-    <row r="207" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="207">
       <c r="H207" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3662,7 +3901,7 @@
         <v/>
       </c>
     </row>
-    <row r="208" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="208">
       <c r="H208" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3672,7 +3911,7 @@
         <v/>
       </c>
     </row>
-    <row r="209" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="209">
       <c r="H209" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3682,7 +3921,7 @@
         <v/>
       </c>
     </row>
-    <row r="210" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="210">
       <c r="H210" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3692,7 +3931,7 @@
         <v/>
       </c>
     </row>
-    <row r="211" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="211">
       <c r="H211" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3702,7 +3941,7 @@
         <v/>
       </c>
     </row>
-    <row r="212" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="212">
       <c r="H212" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3712,7 +3951,7 @@
         <v/>
       </c>
     </row>
-    <row r="213" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="213">
       <c r="H213" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3722,7 +3961,7 @@
         <v/>
       </c>
     </row>
-    <row r="214" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="214">
       <c r="H214" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3732,7 +3971,7 @@
         <v/>
       </c>
     </row>
-    <row r="215" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="215">
       <c r="H215" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3742,7 +3981,7 @@
         <v/>
       </c>
     </row>
-    <row r="216" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="216">
       <c r="H216" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3752,7 +3991,7 @@
         <v/>
       </c>
     </row>
-    <row r="217" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="217">
       <c r="H217" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3762,7 +4001,7 @@
         <v/>
       </c>
     </row>
-    <row r="218" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="218">
       <c r="H218" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3772,7 +4011,7 @@
         <v/>
       </c>
     </row>
-    <row r="219" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="219">
       <c r="H219" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3782,7 +4021,7 @@
         <v/>
       </c>
     </row>
-    <row r="220" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="220">
       <c r="H220" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3792,7 +4031,7 @@
         <v/>
       </c>
     </row>
-    <row r="221" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="221">
       <c r="H221" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3802,7 +4041,7 @@
         <v/>
       </c>
     </row>
-    <row r="222" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="222">
       <c r="H222" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3812,7 +4051,7 @@
         <v/>
       </c>
     </row>
-    <row r="223" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="223">
       <c r="H223" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3822,7 +4061,7 @@
         <v/>
       </c>
     </row>
-    <row r="224" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="224">
       <c r="H224" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3832,7 +4071,7 @@
         <v/>
       </c>
     </row>
-    <row r="225" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="225">
       <c r="H225" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3842,7 +4081,7 @@
         <v/>
       </c>
     </row>
-    <row r="226" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="226">
       <c r="H226" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3852,7 +4091,7 @@
         <v/>
       </c>
     </row>
-    <row r="227" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="227">
       <c r="H227" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3862,7 +4101,7 @@
         <v/>
       </c>
     </row>
-    <row r="228" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="228">
       <c r="H228" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3872,7 +4111,7 @@
         <v/>
       </c>
     </row>
-    <row r="229" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="229">
       <c r="H229" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3882,7 +4121,7 @@
         <v/>
       </c>
     </row>
-    <row r="230" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="230">
       <c r="H230" s="22" t="str">
         <f t="shared" si="8"/>
         <v/>
@@ -3892,7 +4131,7 @@
         <v/>
       </c>
     </row>
-    <row r="231" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="231">
       <c r="H231" s="22" t="str">
         <f t="shared" ref="H231:H234" si="10">IF(OR(D231="",E231=""),"",D231-E231)</f>
         <v/>
@@ -3902,7 +4141,7 @@
         <v/>
       </c>
     </row>
-    <row r="232" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="232">
       <c r="H232" s="22" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -3912,7 +4151,7 @@
         <v/>
       </c>
     </row>
-    <row r="233" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="233">
       <c r="H233" s="22" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -3922,7 +4161,7 @@
         <v/>
       </c>
     </row>
-    <row r="234" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="234">
       <c r="H234" s="22" t="str">
         <f t="shared" si="10"/>
         <v/>
@@ -3932,78 +4171,136 @@
         <v/>
       </c>
     </row>
-    <row r="235" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="235">
       <c r="I235" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="236" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="236">
       <c r="I236" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="237" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="237">
       <c r="I237" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="238" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="238">
       <c r="I238" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="239" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="239">
       <c r="I239" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="240" spans="8:9" x14ac:dyDescent="0.15">
+    <row r="240">
       <c r="I240" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
-    <row r="241" spans="9:9" x14ac:dyDescent="0.15">
+    <row r="241">
       <c r="I241" s="22" t="str">
         <f t="shared" si="11"/>
         <v/>
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="F5:F40 F42:F65521">
-    <cfRule type="cellIs" dxfId="2" priority="2" operator="equal">
-      <formula>"Delayed"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="3" operator="equal">
-      <formula>"Done"</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="4" operator="equal">
-      <formula>"Ongoing"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="F5:F40 F42:F1241" xr:uid="{004C0068-0053-4772-9BC1-008500B300EB}">
-      <formula1>"Planned,Ongoing,Delayed,Done"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="B5:B9 B11:B12 B18:B25 B34 B40:B1241" xr:uid="{00F60079-004C-4143-A0AF-009700D80028}">
-      <formula1>"Requirements,Design,Development,Testing,Preparation,Coordination,Documentation,Interfaces,Delivery"</formula1>
-      <formula2>0</formula2>
-    </dataValidation>
-  </dataValidations>
   <hyperlinks>
-    <hyperlink ref="A6" location="Instructions!A1" display="    See Instructions sheet for usage" xr:uid="{00000000-0004-0000-0100-000000000000}"/>
+    <hyperlink location="Instructions!A1" ref="A6"/>
   </hyperlinks>
-  <printOptions gridLines="1"/>
+  <printOptions headings="0" gridLines="1"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.51181102362204689"/>
-  <pageSetup paperSize="9" scale="70" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup paperSize="9" scale="70" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="landscape" usePrinterDefaults="1" blackAndWhite="0" draft="0" cellComments="none" useFirstPageNumber="0" errors="displayed" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter>
     <oddHeader>&amp;LEdit the Header with Your Team ID&amp;C&amp;F&amp;R&amp;D</oddHeader>
   </headerFooter>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="2" operator="equal" id="{00CB00EE-00EA-4088-A2B0-002700AE00A2}">
+            <xm:f>"Delayed"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFDD0806"/>
+                  <bgColor rgb="FFDD0806"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F5:F40 F42:F65521</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="3" operator="equal" id="{00300051-003E-4EAF-9694-00570008004B}">
+            <xm:f>"Done"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FF006411"/>
+                  <bgColor rgb="FF006411"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F5:F40 F42:F65521</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="cellIs" priority="4" operator="equal" id="{007B00D0-0026-4106-B2BA-00C800A200C3}">
+            <xm:f>"Ongoing"</xm:f>
+            <x14:dxf>
+              <font>
+                <b val="0"/>
+              </font>
+              <fill>
+                <patternFill patternType="solid">
+                  <fgColor rgb="FFFCF305"/>
+                  <bgColor rgb="FFFCF305"/>
+                </patternFill>
+              </fill>
+            </x14:dxf>
+          </x14:cfRule>
+          <xm:sqref>F5:F40 F42:F65521</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="2" disablePrompts="0">
+        <x14:dataValidation xr:uid="{008A00E8-00C9-42E8-9FAD-00B1009800F2}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+          <x14:formula1>
+            <xm:f>"Planned,Ongoing,Delayed,Done"</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>F5:F40 F42:F1241</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation xr:uid="{004500CB-008E-4CFA-9EE8-009F000F0077}" type="list" allowBlank="1" errorStyle="stop" imeMode="noControl" operator="between" showDropDown="0" showErrorMessage="1" showInputMessage="0">
+          <x14:formula1>
+            <xm:f>"Requirements,Design,Development,Testing,Preparation,Coordination,Documentation,Interfaces,Delivery"</xm:f>
+          </x14:formula1>
+          <x14:formula2>
+            <xm:f>0</xm:f>
+          </x14:formula2>
+          <xm:sqref>B5:B9 B11:B12 B18:B25 B34 B40:B1241</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>